<commit_message>
conf scheduling: prohibited and undesired timeslot and room tags
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="140">
   <si>
     <t>Conference name</t>
   </si>
@@ -59,18 +59,36 @@
     <t>Soft penalty per missing preferred tag in a talk's timeslot</t>
   </si>
   <si>
+    <t>Speaker undesired timeslot tag</t>
+  </si>
+  <si>
+    <t>Soft penalty per undesired tag in a talk's timeslot</t>
+  </si>
+  <si>
     <t>Talk preferred timeslot tag</t>
   </si>
   <si>
+    <t>Talk undesired timeslot tag</t>
+  </si>
+  <si>
     <t>Speaker preferred room tag</t>
   </si>
   <si>
     <t>Soft penalty per missing preferred tag in a talk's room</t>
   </si>
   <si>
+    <t>Speaker undesired room tag</t>
+  </si>
+  <si>
+    <t>Soft penalty per undesired tag in a talk's room</t>
+  </si>
+  <si>
     <t>Talk preferred room tag</t>
   </si>
   <si>
+    <t>Talk undesired room tag</t>
+  </si>
+  <si>
     <t>Day</t>
   </si>
   <si>
@@ -182,10 +200,22 @@
     <t>Preferred timeslot tags</t>
   </si>
   <si>
+    <t>Prohibited timeslot tags</t>
+  </si>
+  <si>
+    <t>Undesired timeslot tags</t>
+  </si>
+  <si>
     <t>Required room tags</t>
   </si>
   <si>
     <t>Preferred room tags</t>
+  </si>
+  <si>
+    <t>Prohibited room tags</t>
+  </si>
+  <si>
+    <t>Undesired room tags</t>
   </si>
   <si>
     <t>Amy Cole</t>
@@ -482,9 +512,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="29.0859375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.80859375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="70.88671875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="33.8671875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.33203125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="81.296875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -559,18 +589,18 @@
         <v>10.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="n">
         <v>10.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -581,7 +611,51 @@
         <v>10.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -600,130 +674,130 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="15.99609375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="6.0859375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="6.0859375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="9.41796875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="5.1484375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="16.14453125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="6.3984375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="6.32421875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="10.78515625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="6.078125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -742,196 +816,196 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.48828125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="25.6328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="7.109375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="26.3125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.6171875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -953,512 +1027,684 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="21.69921875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="22.09765625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="19.07421875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="19.47265625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="11.9453125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="24.85546875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="25.390625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="26.30859375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="26.0234375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="21.671875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="22.20703125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="23.125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="22.84375" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.6171875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K3" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K4" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="L5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K6" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="L6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K7" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="L7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K8" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="L8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I9" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J9" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K9" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="L9" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" t="s">
+        <v>32</v>
+      </c>
+      <c r="O9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="H10" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I10" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J10" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K10" t="s">
-        <v>26</v>
+        <v>51</v>
+      </c>
+      <c r="L10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10" t="s">
+        <v>32</v>
+      </c>
+      <c r="N10" t="s">
+        <v>32</v>
+      </c>
+      <c r="O10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" t="s">
+        <v>32</v>
       </c>
       <c r="I11" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" t="s">
-        <v>26</v>
-      </c>
-      <c r="K11" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11" t="s">
+        <v>32</v>
+      </c>
+      <c r="N11" t="s">
+        <v>32</v>
+      </c>
+      <c r="O11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="H12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K12" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="L12" t="s">
+        <v>32</v>
+      </c>
+      <c r="M12" t="s">
+        <v>32</v>
+      </c>
+      <c r="N12" t="s">
+        <v>32</v>
+      </c>
+      <c r="O12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K13" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="L13" t="s">
+        <v>32</v>
+      </c>
+      <c r="M13" t="s">
+        <v>32</v>
+      </c>
+      <c r="N13" t="s">
+        <v>32</v>
+      </c>
+      <c r="O13" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G14" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H14" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I14" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J14" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K14" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="L14" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" t="s">
+        <v>32</v>
+      </c>
+      <c r="N14" t="s">
+        <v>32</v>
+      </c>
+      <c r="O14" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="J1:O1"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1475,972 +1721,1204 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="32.125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="9.41796875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="19.3515625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="14.375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="9.7109375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="18.9453125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="21.69921875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="22.09765625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="19.07421875" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="19.47265625" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="14.578125" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="15.99609375" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="6.0859375" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="6.0859375" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="6.44921875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="6.34765625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="33.1015625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.78515625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="19.83203125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="14.55078125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="11.3046875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="19.76171875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="24.85546875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="25.390625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="26.30859375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="26.0234375" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="21.671875" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="22.20703125" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="23.125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="22.84375" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="16.65234375" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" width="16.14453125" customWidth="true" bestFit="true"/>
+    <col min="18" max="18" width="6.3984375" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" width="6.32421875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="7.02734375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>76</v>
+        <v>84</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J2" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" t="b">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" t="b">
         <v>0</v>
       </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" t="s">
-        <v>26</v>
+      <c r="Q2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G3" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J3" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="K3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" t="b">
+        <v>32</v>
+      </c>
+      <c r="L3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" t="b">
         <v>0</v>
       </c>
-      <c r="M3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" t="s">
-        <v>26</v>
+      <c r="Q3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="E4" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G4" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" t="b">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" t="b">
         <v>0</v>
       </c>
-      <c r="M4" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4" t="s">
-        <v>26</v>
+      <c r="Q4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4" t="s">
+        <v>32</v>
+      </c>
+      <c r="S4" t="s">
+        <v>32</v>
+      </c>
+      <c r="T4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="F5" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" t="b">
+        <v>32</v>
+      </c>
+      <c r="L5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" t="b">
         <v>0</v>
       </c>
-      <c r="M5" t="s">
-        <v>26</v>
-      </c>
-      <c r="N5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5" t="s">
-        <v>26</v>
+      <c r="Q5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" t="b">
+        <v>32</v>
+      </c>
+      <c r="L6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P6" t="b">
         <v>0</v>
       </c>
-      <c r="M6" t="s">
-        <v>26</v>
-      </c>
-      <c r="N6" t="s">
-        <v>26</v>
-      </c>
-      <c r="O6" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6" t="s">
-        <v>26</v>
+      <c r="Q6" t="s">
+        <v>32</v>
+      </c>
+      <c r="R6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S6" t="s">
+        <v>32</v>
+      </c>
+      <c r="T6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" t="s">
+        <v>32</v>
+      </c>
+      <c r="P7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G7" t="s">
-        <v>98</v>
-      </c>
-      <c r="H7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="M7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" t="s">
-        <v>23</v>
-      </c>
-      <c r="O7" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" t="s">
-        <v>43</v>
+      <c r="R7" t="s">
+        <v>29</v>
+      </c>
+      <c r="S7" t="s">
+        <v>33</v>
+      </c>
+      <c r="T7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G8" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="H8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L8" t="b">
+        <v>32</v>
+      </c>
+      <c r="L8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" t="b">
         <v>0</v>
       </c>
-      <c r="M8" t="s">
-        <v>26</v>
-      </c>
-      <c r="N8" t="s">
-        <v>26</v>
-      </c>
-      <c r="O8" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" t="s">
-        <v>26</v>
+      <c r="Q8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T8" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G9" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I9" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J9" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L9" t="b">
+        <v>32</v>
+      </c>
+      <c r="L9" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" t="s">
+        <v>32</v>
+      </c>
+      <c r="O9" t="s">
+        <v>32</v>
+      </c>
+      <c r="P9" t="b">
         <v>0</v>
       </c>
-      <c r="M9" t="s">
-        <v>26</v>
-      </c>
-      <c r="N9" t="s">
-        <v>26</v>
-      </c>
-      <c r="O9" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" t="s">
-        <v>26</v>
+      <c r="Q9" t="s">
+        <v>32</v>
+      </c>
+      <c r="R9" t="s">
+        <v>32</v>
+      </c>
+      <c r="S9" t="s">
+        <v>32</v>
+      </c>
+      <c r="T9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G10" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="H10" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I10" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J10" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K10" t="s">
-        <v>26</v>
-      </c>
-      <c r="L10" t="b">
+        <v>32</v>
+      </c>
+      <c r="L10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10" t="s">
+        <v>32</v>
+      </c>
+      <c r="N10" t="s">
+        <v>32</v>
+      </c>
+      <c r="O10" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" t="b">
         <v>0</v>
       </c>
-      <c r="M10" t="s">
-        <v>26</v>
-      </c>
-      <c r="N10" t="s">
-        <v>26</v>
-      </c>
-      <c r="O10" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" t="s">
-        <v>26</v>
+      <c r="Q10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R10" t="s">
+        <v>32</v>
+      </c>
+      <c r="S10" t="s">
+        <v>32</v>
+      </c>
+      <c r="T10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G11" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="H11" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I11" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J11" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K11" t="s">
-        <v>26</v>
-      </c>
-      <c r="L11" t="b">
+        <v>32</v>
+      </c>
+      <c r="L11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11" t="s">
+        <v>32</v>
+      </c>
+      <c r="N11" t="s">
+        <v>32</v>
+      </c>
+      <c r="O11" t="s">
+        <v>32</v>
+      </c>
+      <c r="P11" t="b">
         <v>0</v>
       </c>
-      <c r="M11" t="s">
-        <v>26</v>
-      </c>
-      <c r="N11" t="s">
-        <v>26</v>
-      </c>
-      <c r="O11" t="s">
-        <v>26</v>
-      </c>
-      <c r="P11" t="s">
-        <v>26</v>
+      <c r="Q11" t="s">
+        <v>32</v>
+      </c>
+      <c r="R11" t="s">
+        <v>32</v>
+      </c>
+      <c r="S11" t="s">
+        <v>32</v>
+      </c>
+      <c r="T11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F12" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="H12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K12" t="s">
-        <v>26</v>
-      </c>
-      <c r="L12" t="b">
+        <v>32</v>
+      </c>
+      <c r="L12" t="s">
+        <v>32</v>
+      </c>
+      <c r="M12" t="s">
+        <v>32</v>
+      </c>
+      <c r="N12" t="s">
+        <v>32</v>
+      </c>
+      <c r="O12" t="s">
+        <v>32</v>
+      </c>
+      <c r="P12" t="b">
         <v>0</v>
       </c>
-      <c r="M12" t="s">
-        <v>26</v>
-      </c>
-      <c r="N12" t="s">
-        <v>26</v>
-      </c>
-      <c r="O12" t="s">
-        <v>26</v>
-      </c>
-      <c r="P12" t="s">
-        <v>26</v>
+      <c r="Q12" t="s">
+        <v>32</v>
+      </c>
+      <c r="R12" t="s">
+        <v>32</v>
+      </c>
+      <c r="S12" t="s">
+        <v>32</v>
+      </c>
+      <c r="T12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G13" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="H13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K13" t="s">
-        <v>26</v>
-      </c>
-      <c r="L13" t="b">
+        <v>32</v>
+      </c>
+      <c r="L13" t="s">
+        <v>32</v>
+      </c>
+      <c r="M13" t="s">
+        <v>32</v>
+      </c>
+      <c r="N13" t="s">
+        <v>32</v>
+      </c>
+      <c r="O13" t="s">
+        <v>32</v>
+      </c>
+      <c r="P13" t="b">
         <v>0</v>
       </c>
-      <c r="M13" t="s">
-        <v>26</v>
-      </c>
-      <c r="N13" t="s">
-        <v>26</v>
-      </c>
-      <c r="O13" t="s">
-        <v>26</v>
-      </c>
-      <c r="P13" t="s">
-        <v>26</v>
+      <c r="Q13" t="s">
+        <v>32</v>
+      </c>
+      <c r="R13" t="s">
+        <v>32</v>
+      </c>
+      <c r="S13" t="s">
+        <v>32</v>
+      </c>
+      <c r="T13" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G14" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="H14" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I14" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J14" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K14" t="s">
-        <v>26</v>
-      </c>
-      <c r="L14" t="b">
+        <v>32</v>
+      </c>
+      <c r="L14" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" t="s">
+        <v>32</v>
+      </c>
+      <c r="N14" t="s">
+        <v>32</v>
+      </c>
+      <c r="O14" t="s">
+        <v>32</v>
+      </c>
+      <c r="P14" t="b">
         <v>0</v>
       </c>
-      <c r="M14" t="s">
-        <v>26</v>
-      </c>
-      <c r="N14" t="s">
-        <v>26</v>
-      </c>
-      <c r="O14" t="s">
-        <v>26</v>
-      </c>
-      <c r="P14" t="s">
-        <v>26</v>
+      <c r="Q14" t="s">
+        <v>32</v>
+      </c>
+      <c r="R14" t="s">
+        <v>32</v>
+      </c>
+      <c r="S14" t="s">
+        <v>32</v>
+      </c>
+      <c r="T14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F15" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G15" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="H15" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I15" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J15" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K15" t="s">
-        <v>26</v>
-      </c>
-      <c r="L15" t="b">
+        <v>32</v>
+      </c>
+      <c r="L15" t="s">
+        <v>32</v>
+      </c>
+      <c r="M15" t="s">
+        <v>32</v>
+      </c>
+      <c r="N15" t="s">
+        <v>32</v>
+      </c>
+      <c r="O15" t="s">
+        <v>32</v>
+      </c>
+      <c r="P15" t="b">
         <v>0</v>
       </c>
-      <c r="M15" t="s">
-        <v>26</v>
-      </c>
-      <c r="N15" t="s">
-        <v>26</v>
-      </c>
-      <c r="O15" t="s">
-        <v>26</v>
-      </c>
-      <c r="P15" t="s">
-        <v>26</v>
+      <c r="Q15" t="s">
+        <v>32</v>
+      </c>
+      <c r="R15" t="s">
+        <v>32</v>
+      </c>
+      <c r="S15" t="s">
+        <v>32</v>
+      </c>
+      <c r="T15" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B16" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F16" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G16" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="H16" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I16" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J16" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K16" t="s">
-        <v>26</v>
-      </c>
-      <c r="L16" t="b">
+        <v>32</v>
+      </c>
+      <c r="L16" t="s">
+        <v>32</v>
+      </c>
+      <c r="M16" t="s">
+        <v>32</v>
+      </c>
+      <c r="N16" t="s">
+        <v>32</v>
+      </c>
+      <c r="O16" t="s">
+        <v>32</v>
+      </c>
+      <c r="P16" t="b">
         <v>0</v>
       </c>
-      <c r="M16" t="s">
-        <v>26</v>
-      </c>
-      <c r="N16" t="s">
-        <v>26</v>
-      </c>
-      <c r="O16" t="s">
-        <v>26</v>
-      </c>
-      <c r="P16" t="s">
-        <v>26</v>
+      <c r="Q16" t="s">
+        <v>32</v>
+      </c>
+      <c r="R16" t="s">
+        <v>32</v>
+      </c>
+      <c r="S16" t="s">
+        <v>32</v>
+      </c>
+      <c r="T16" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G17" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="H17" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I17" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J17" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K17" t="s">
-        <v>26</v>
-      </c>
-      <c r="L17" t="b">
+        <v>32</v>
+      </c>
+      <c r="L17" t="s">
+        <v>32</v>
+      </c>
+      <c r="M17" t="s">
+        <v>32</v>
+      </c>
+      <c r="N17" t="s">
+        <v>32</v>
+      </c>
+      <c r="O17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P17" t="b">
         <v>0</v>
       </c>
-      <c r="M17" t="s">
-        <v>26</v>
-      </c>
-      <c r="N17" t="s">
-        <v>26</v>
-      </c>
-      <c r="O17" t="s">
-        <v>26</v>
-      </c>
-      <c r="P17" t="s">
-        <v>26</v>
+      <c r="Q17" t="s">
+        <v>32</v>
+      </c>
+      <c r="R17" t="s">
+        <v>32</v>
+      </c>
+      <c r="S17" t="s">
+        <v>32</v>
+      </c>
+      <c r="T17" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="B18" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G18" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="H18" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I18" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J18" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K18" t="s">
-        <v>26</v>
-      </c>
-      <c r="L18" t="b">
+        <v>32</v>
+      </c>
+      <c r="L18" t="s">
+        <v>32</v>
+      </c>
+      <c r="M18" t="s">
+        <v>32</v>
+      </c>
+      <c r="N18" t="s">
+        <v>32</v>
+      </c>
+      <c r="O18" t="s">
+        <v>32</v>
+      </c>
+      <c r="P18" t="b">
         <v>0</v>
       </c>
-      <c r="M18" t="s">
-        <v>26</v>
-      </c>
-      <c r="N18" t="s">
-        <v>26</v>
-      </c>
-      <c r="O18" t="s">
-        <v>26</v>
-      </c>
-      <c r="P18" t="s">
-        <v>26</v>
+      <c r="Q18" t="s">
+        <v>32</v>
+      </c>
+      <c r="R18" t="s">
+        <v>32</v>
+      </c>
+      <c r="S18" t="s">
+        <v>32</v>
+      </c>
+      <c r="T18" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="B19" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G19" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="H19" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I19" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J19" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K19" t="s">
-        <v>26</v>
-      </c>
-      <c r="L19" t="b">
+        <v>32</v>
+      </c>
+      <c r="L19" t="s">
+        <v>32</v>
+      </c>
+      <c r="M19" t="s">
+        <v>32</v>
+      </c>
+      <c r="N19" t="s">
+        <v>32</v>
+      </c>
+      <c r="O19" t="s">
+        <v>32</v>
+      </c>
+      <c r="P19" t="b">
         <v>0</v>
       </c>
-      <c r="M19" t="s">
-        <v>26</v>
-      </c>
-      <c r="N19" t="s">
-        <v>26</v>
-      </c>
-      <c r="O19" t="s">
-        <v>26</v>
-      </c>
-      <c r="P19" t="s">
-        <v>26</v>
+      <c r="Q19" t="s">
+        <v>32</v>
+      </c>
+      <c r="R19" t="s">
+        <v>32</v>
+      </c>
+      <c r="S19" t="s">
+        <v>32</v>
+      </c>
+      <c r="T19" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2459,82 +2937,82 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.71875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="12.203125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="13.6171875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2557,59 +3035,59 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.23828125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="11.94140625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="13.6171875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
conf scheduling: add audience level and content tags + change speakers column order
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
@@ -13,12 +13,13 @@
     <sheet name="Talks" r:id="rId7" sheetId="5"/>
     <sheet name="Theme view" r:id="rId8" sheetId="6"/>
     <sheet name="Sector view" r:id="rId9" sheetId="7"/>
+    <sheet name="Speaker view" r:id="rId10" sheetId="8"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="165">
   <si>
     <t>Conference name</t>
   </si>
@@ -173,271 +174,346 @@
     <t>Large, Recorded</t>
   </si>
   <si>
+    <t>S06</t>
+  </si>
+  <si>
+    <t>R 2</t>
+  </si>
+  <si>
+    <t>R 3</t>
+  </si>
+  <si>
+    <t>Recorded</t>
+  </si>
+  <si>
+    <t>R 4</t>
+  </si>
+  <si>
+    <t>R 5</t>
+  </si>
+  <si>
+    <t>Lab_room, Large, Recorded</t>
+  </si>
+  <si>
+    <t>Required timeslot tags</t>
+  </si>
+  <si>
+    <t>Preferred timeslot tags</t>
+  </si>
+  <si>
+    <t>Prohibited timeslot tags</t>
+  </si>
+  <si>
+    <t>Undesired timeslot tags</t>
+  </si>
+  <si>
+    <t>Required room tags</t>
+  </si>
+  <si>
+    <t>Preferred room tags</t>
+  </si>
+  <si>
+    <t>Prohibited room tags</t>
+  </si>
+  <si>
+    <t>Undesired room tags</t>
+  </si>
+  <si>
+    <t>Amy Cole</t>
+  </si>
+  <si>
+    <t>Beth Fox</t>
+  </si>
+  <si>
+    <t>Chad Green</t>
+  </si>
+  <si>
+    <t>Dan Jones</t>
+  </si>
+  <si>
+    <t>Elsa King</t>
+  </si>
+  <si>
+    <t>Flo Li</t>
+  </si>
+  <si>
+    <t>Gus Poe</t>
+  </si>
+  <si>
+    <t>Hugo Rye</t>
+  </si>
+  <si>
+    <t>Ivy Smith</t>
+  </si>
+  <si>
+    <t>Jay Watt</t>
+  </si>
+  <si>
+    <t>Amy Fox</t>
+  </si>
+  <si>
+    <t>Beth Green</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Speakers</t>
+  </si>
+  <si>
+    <t>Theme tags</t>
+  </si>
+  <si>
+    <t>Sector tags</t>
+  </si>
+  <si>
+    <t>Audience level</t>
+  </si>
+  <si>
+    <t>Content tags</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Pinned by user</t>
+  </si>
+  <si>
+    <t>Timeslot day</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>S00</t>
+  </si>
+  <si>
+    <t>Hands on real-time OpenShift</t>
+  </si>
+  <si>
+    <t>Cloud</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>OpenShift, Kubernetes</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>Lab_room</t>
+  </si>
+  <si>
+    <t>S01</t>
+  </si>
+  <si>
+    <t>Advanced containerized WildFly</t>
+  </si>
+  <si>
+    <t>Big Data</t>
+  </si>
+  <si>
+    <t>WildFly</t>
+  </si>
+  <si>
+    <t>S02</t>
+  </si>
+  <si>
+    <t>Learn virtualized Spring</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>S03</t>
+  </si>
+  <si>
+    <t>Intro to serverless Drools</t>
+  </si>
+  <si>
+    <t>Culture</t>
+  </si>
+  <si>
+    <t>Drools</t>
+  </si>
+  <si>
+    <t>S04</t>
+  </si>
+  <si>
+    <t>Discover AI-driven OptaPlanner</t>
+  </si>
+  <si>
+    <t>Elsa King, Flo Li</t>
+  </si>
+  <si>
+    <t>IoT</t>
+  </si>
+  <si>
+    <t>OptaPlanner</t>
+  </si>
+  <si>
     <t>S05</t>
   </si>
   <si>
-    <t>R 2</t>
-  </si>
-  <si>
-    <t>R 3</t>
-  </si>
-  <si>
-    <t>Recorded</t>
-  </si>
-  <si>
-    <t>R 4</t>
-  </si>
-  <si>
-    <t>R 5</t>
-  </si>
-  <si>
-    <t>Lab_room, Large, Recorded</t>
-  </si>
-  <si>
-    <t>Required timeslot tags</t>
-  </si>
-  <si>
-    <t>Preferred timeslot tags</t>
-  </si>
-  <si>
-    <t>Prohibited timeslot tags</t>
-  </si>
-  <si>
-    <t>Undesired timeslot tags</t>
-  </si>
-  <si>
-    <t>Required room tags</t>
-  </si>
-  <si>
-    <t>Preferred room tags</t>
-  </si>
-  <si>
-    <t>Prohibited room tags</t>
-  </si>
-  <si>
-    <t>Undesired room tags</t>
-  </si>
-  <si>
-    <t>Amy Cole</t>
-  </si>
-  <si>
-    <t>Beth Fox</t>
-  </si>
-  <si>
-    <t>Chad Green</t>
-  </si>
-  <si>
-    <t>Dan Jones</t>
-  </si>
-  <si>
-    <t>Elsa King</t>
-  </si>
-  <si>
-    <t>Flo Li</t>
-  </si>
-  <si>
-    <t>Gus Poe</t>
-  </si>
-  <si>
-    <t>Hugo Rye</t>
-  </si>
-  <si>
-    <t>Ivy Smith</t>
-  </si>
-  <si>
-    <t>Jay Watt</t>
-  </si>
-  <si>
-    <t>Amy Fox</t>
-  </si>
-  <si>
-    <t>Beth Green</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Theme tags</t>
-  </si>
-  <si>
-    <t>Sector tags</t>
-  </si>
-  <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>Speakers</t>
-  </si>
-  <si>
-    <t>Pinned by user</t>
-  </si>
-  <si>
-    <t>Timeslot day</t>
-  </si>
-  <si>
-    <t>Room</t>
-  </si>
-  <si>
-    <t>S00</t>
-  </si>
-  <si>
-    <t>Hands on real-time OpenShift</t>
-  </si>
-  <si>
-    <t>Mobile</t>
-  </si>
-  <si>
-    <t>en</t>
+    <t>Mastering machine learning jBPM</t>
+  </si>
+  <si>
+    <t>Gus Poe, Hugo Rye</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>jBPM</t>
+  </si>
+  <si>
+    <t>Tuning IOT-driven Camel</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>Camel</t>
+  </si>
+  <si>
+    <t>S07</t>
+  </si>
+  <si>
+    <t>Building deep learning XStream</t>
+  </si>
+  <si>
+    <t>XStream</t>
+  </si>
+  <si>
+    <t>S08</t>
+  </si>
+  <si>
+    <t>Securing scalable Docker</t>
+  </si>
+  <si>
+    <t>Amy Fox, Beth Green</t>
+  </si>
+  <si>
+    <t>Modern Web</t>
+  </si>
+  <si>
+    <t>Docker</t>
+  </si>
+  <si>
+    <t>S09</t>
+  </si>
+  <si>
+    <t>Debug enterprise Hibernate</t>
+  </si>
+  <si>
+    <t>Hibernate</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>Prepare for streaming GWT</t>
+  </si>
+  <si>
+    <t>Beth Fox, Chad Green</t>
+  </si>
+  <si>
+    <t>Security, Cloud</t>
+  </si>
+  <si>
+    <t>GWT</t>
+  </si>
+  <si>
+    <t>S11</t>
+  </si>
+  <si>
+    <t>Understand mobile Errai</t>
+  </si>
+  <si>
+    <t>Errai</t>
+  </si>
+  <si>
+    <t>S12</t>
+  </si>
+  <si>
+    <t>Applying modern Angular</t>
+  </si>
+  <si>
+    <t>Angular</t>
+  </si>
+  <si>
+    <t>S13</t>
+  </si>
+  <si>
+    <t>Grok distributed Weld</t>
+  </si>
+  <si>
+    <t>Weld</t>
+  </si>
+  <si>
+    <t>S14</t>
+  </si>
+  <si>
+    <t>Troubleshooting reliable RestEasy</t>
+  </si>
+  <si>
+    <t>Security, Mobile</t>
+  </si>
+  <si>
+    <t>RestEasy</t>
+  </si>
+  <si>
+    <t>S15</t>
+  </si>
+  <si>
+    <t>Using secure Android</t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>S16</t>
+  </si>
+  <si>
+    <t>Deliver stable Tensorflow</t>
+  </si>
+  <si>
+    <t>Cloud, Modern Web</t>
+  </si>
+  <si>
+    <t>Tensorflow</t>
+  </si>
+  <si>
+    <t>S17</t>
+  </si>
+  <si>
+    <t>Implement platform-independent VertX</t>
   </si>
   <si>
     <t>Amy Cole, Beth Fox</t>
   </si>
   <si>
-    <t>Lab_room</t>
-  </si>
-  <si>
-    <t>S01</t>
-  </si>
-  <si>
-    <t>Advanced containerized WildFly</t>
-  </si>
-  <si>
-    <t>Big Data</t>
-  </si>
-  <si>
-    <t>S02</t>
-  </si>
-  <si>
-    <t>Learn virtualized Spring</t>
-  </si>
-  <si>
-    <t>Artificial Intelligence</t>
-  </si>
-  <si>
-    <t>Transportation</t>
-  </si>
-  <si>
-    <t>Dan Jones, Elsa King</t>
-  </si>
-  <si>
-    <t>S03</t>
-  </si>
-  <si>
-    <t>Intro to serverless Drools</t>
-  </si>
-  <si>
-    <t>Mobile, Big Data</t>
-  </si>
-  <si>
-    <t>S04</t>
-  </si>
-  <si>
-    <t>Discover AI-driven OptaPlanner</t>
-  </si>
-  <si>
-    <t>Cloud</t>
-  </si>
-  <si>
-    <t>Mastering machine learning jBPM</t>
-  </si>
-  <si>
-    <t>Hugo Rye, Ivy Smith</t>
-  </si>
-  <si>
-    <t>S06</t>
-  </si>
-  <si>
-    <t>Tuning IOT-driven Camel</t>
-  </si>
-  <si>
-    <t>Security</t>
-  </si>
-  <si>
-    <t>Jay Watt, Amy Fox</t>
-  </si>
-  <si>
-    <t>S07</t>
-  </si>
-  <si>
-    <t>Building deep learning XStream</t>
-  </si>
-  <si>
-    <t>S08</t>
-  </si>
-  <si>
-    <t>Securing scalable Docker</t>
-  </si>
-  <si>
-    <t>IoT</t>
-  </si>
-  <si>
-    <t>S09</t>
-  </si>
-  <si>
-    <t>Debug enterprise JUnit</t>
-  </si>
-  <si>
-    <t>Culture, Security</t>
-  </si>
-  <si>
-    <t>S10</t>
-  </si>
-  <si>
-    <t>Hands on real-time WildFly</t>
-  </si>
-  <si>
-    <t>S11</t>
-  </si>
-  <si>
-    <t>Advanced containerized Spring</t>
-  </si>
-  <si>
-    <t>S12</t>
-  </si>
-  <si>
-    <t>Learn virtualized Drools</t>
-  </si>
-  <si>
-    <t>S13</t>
-  </si>
-  <si>
-    <t>Intro to serverless OptaPlanner</t>
-  </si>
-  <si>
-    <t>S14</t>
-  </si>
-  <si>
-    <t>Discover AI-driven jBPM</t>
-  </si>
-  <si>
-    <t>S15</t>
-  </si>
-  <si>
-    <t>Mastering machine learning Camel</t>
-  </si>
-  <si>
-    <t>Mobile, Security</t>
-  </si>
-  <si>
-    <t>S16</t>
-  </si>
-  <si>
-    <t>Tuning IOT-driven XStream</t>
-  </si>
-  <si>
-    <t>S17</t>
-  </si>
-  <si>
-    <t>Building deep learning Docker</t>
+    <t>Middleware, Modern Web</t>
+  </si>
+  <si>
+    <t>VertX</t>
   </si>
   <si>
     <t>Theme tag</t>
   </si>
   <si>
     <t>Sector tag</t>
+  </si>
+  <si>
+    <t>Speaker</t>
   </si>
 </sst>
 </file>
@@ -459,7 +535,7 @@
       <b val="true"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -479,6 +555,16 @@
         <fgColor rgb="AD7FA8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="EF2929"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FCAF3E"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -492,11 +578,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -512,9 +600,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="33.8671875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.33203125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="81.296875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="29.5" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.80859375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="70.88671875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -674,11 +762,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.14453125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="6.3984375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="6.32421875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="10.78515625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="6.078125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="15.99609375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="6.0859375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="6.0859375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="9.41796875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="5.1484375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -816,14 +904,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="7.109375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="26.3125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="6.48828125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="25.6328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="11.86328125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1027,21 +1115,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="11.9453125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="24.85546875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="25.390625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="26.30859375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="26.0234375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="21.671875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="22.20703125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="23.125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="22.84375" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="11.5703125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="21.69921875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="22.09765625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="23.01171875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="22.7734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="19.07421875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="19.47265625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="20.3828125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="20.1484375" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="11.86328125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1499,7 +1587,7 @@
         <v>32</v>
       </c>
       <c r="K10" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="L10" t="s">
         <v>32</v>
@@ -1721,26 +1809,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="33.1015625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.78515625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="19.83203125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="14.55078125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="11.3046875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="19.76171875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="24.85546875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="25.390625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="26.30859375" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="26.0234375" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="21.671875" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="22.20703125" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="23.125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="22.84375" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="16.65234375" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" width="16.14453125" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" width="6.3984375" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" width="6.32421875" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="7.02734375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="36.7734375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="9.41796875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="20.421875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="24.78515625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="12.33984375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.4375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="21.28515625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="9.7109375" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="21.69921875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="22.09765625" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="23.01171875" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="22.7734375" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="19.07421875" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="19.47265625" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="20.3828125" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" width="20.1484375" customWidth="true" bestFit="true"/>
+    <col min="18" max="18" width="14.578125" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" width="15.99609375" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="6.0859375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="6.0859375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="6.44921875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1766,72 +1856,78 @@
         <v>83</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="R1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>86</v>
+      <c r="V1" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G2" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2.0</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="I2" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="J2" t="s">
         <v>32</v>
@@ -1840,122 +1936,134 @@
         <v>32</v>
       </c>
       <c r="L2" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
         <v>32</v>
       </c>
       <c r="N2" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="O2" t="s">
         <v>32</v>
       </c>
-      <c r="P2" t="b">
+      <c r="P2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" t="b">
         <v>0</v>
       </c>
-      <c r="Q2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R2" t="s">
-        <v>32</v>
-      </c>
       <c r="S2" t="s">
         <v>32</v>
       </c>
       <c r="T2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
         <v>31</v>
       </c>
       <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I3" t="s">
+        <v>94</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" t="s">
         <v>95</v>
       </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" t="s">
-        <v>92</v>
-      </c>
-      <c r="M3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" t="s">
-        <v>32</v>
-      </c>
       <c r="O3" t="s">
         <v>32</v>
       </c>
-      <c r="P3" t="b">
+      <c r="P3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" t="b">
         <v>0</v>
       </c>
-      <c r="Q3" t="s">
-        <v>32</v>
-      </c>
-      <c r="R3" t="s">
-        <v>32</v>
-      </c>
       <c r="S3" t="s">
         <v>32</v>
       </c>
       <c r="T3" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" t="s">
+        <v>32</v>
+      </c>
+      <c r="V3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C4" t="s">
         <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G4" t="s">
-        <v>100</v>
+        <v>32</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3.0</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="J4" t="s">
         <v>32</v>
@@ -1975,49 +2083,55 @@
       <c r="O4" t="s">
         <v>32</v>
       </c>
-      <c r="P4" t="b">
+      <c r="P4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4" t="b">
         <v>0</v>
       </c>
-      <c r="Q4" t="s">
-        <v>32</v>
-      </c>
-      <c r="R4" t="s">
-        <v>32</v>
-      </c>
       <c r="S4" t="s">
         <v>32</v>
       </c>
       <c r="T4" t="s">
+        <v>32</v>
+      </c>
+      <c r="U4" t="s">
+        <v>32</v>
+      </c>
+      <c r="V4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C5" t="s">
         <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="F5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G5" t="s">
-        <v>71</v>
+        <v>32</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2.0</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="I5" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="J5" t="s">
         <v>32</v>
@@ -2037,49 +2151,55 @@
       <c r="O5" t="s">
         <v>32</v>
       </c>
-      <c r="P5" t="b">
+      <c r="P5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R5" t="b">
         <v>0</v>
       </c>
-      <c r="Q5" t="s">
-        <v>32</v>
-      </c>
-      <c r="R5" t="s">
-        <v>32</v>
-      </c>
       <c r="S5" t="s">
         <v>32</v>
       </c>
       <c r="T5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>111</v>
       </c>
       <c r="F6" t="s">
-        <v>90</v>
-      </c>
-      <c r="G6" t="s">
-        <v>72</v>
+        <v>32</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3.0</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>112</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="J6" t="s">
         <v>32</v>
@@ -2099,49 +2219,55 @@
       <c r="O6" t="s">
         <v>32</v>
       </c>
-      <c r="P6" t="b">
+      <c r="P6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>32</v>
+      </c>
+      <c r="R6" t="b">
         <v>0</v>
       </c>
-      <c r="Q6" t="s">
-        <v>32</v>
-      </c>
-      <c r="R6" t="s">
-        <v>32</v>
-      </c>
       <c r="S6" t="s">
         <v>32</v>
       </c>
       <c r="T6" t="s">
+        <v>32</v>
+      </c>
+      <c r="U6" t="s">
+        <v>32</v>
+      </c>
+      <c r="V6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G7" t="s">
-        <v>108</v>
+        <v>32</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1.0</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>117</v>
       </c>
       <c r="I7" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="J7" t="s">
         <v>32</v>
@@ -2161,49 +2287,55 @@
       <c r="O7" t="s">
         <v>32</v>
       </c>
-      <c r="P7" s="3" t="b">
-        <v>1</v>
+      <c r="P7" t="s">
+        <v>32</v>
       </c>
       <c r="Q7" t="s">
-        <v>28</v>
-      </c>
-      <c r="R7" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="R7" t="b">
+        <v>0</v>
       </c>
       <c r="S7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T7" t="s">
-        <v>49</v>
+        <v>32</v>
+      </c>
+      <c r="U7" t="s">
+        <v>32</v>
+      </c>
+      <c r="V7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C8" t="s">
         <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="F8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G8" t="s">
-        <v>112</v>
+        <v>32</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.0</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="I8" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="J8" t="s">
         <v>32</v>
@@ -2223,49 +2355,55 @@
       <c r="O8" t="s">
         <v>32</v>
       </c>
-      <c r="P8" t="b">
-        <v>0</v>
+      <c r="P8" t="s">
+        <v>32</v>
       </c>
       <c r="Q8" t="s">
         <v>32</v>
       </c>
-      <c r="R8" t="s">
-        <v>32</v>
+      <c r="R8" s="3" t="b">
+        <v>1</v>
       </c>
       <c r="S8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="T8" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+      <c r="U8" t="s">
+        <v>33</v>
+      </c>
+      <c r="V8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="C9" t="s">
         <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>111</v>
       </c>
       <c r="F9" t="s">
-        <v>90</v>
-      </c>
-      <c r="G9" t="s">
-        <v>77</v>
+        <v>32</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2.0</v>
       </c>
       <c r="H9" t="s">
-        <v>32</v>
+        <v>123</v>
       </c>
       <c r="I9" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="J9" t="s">
         <v>32</v>
@@ -2285,49 +2423,55 @@
       <c r="O9" t="s">
         <v>32</v>
       </c>
-      <c r="P9" t="b">
+      <c r="P9" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>32</v>
+      </c>
+      <c r="R9" t="b">
         <v>0</v>
       </c>
-      <c r="Q9" t="s">
-        <v>32</v>
-      </c>
-      <c r="R9" t="s">
-        <v>32</v>
-      </c>
       <c r="S9" t="s">
         <v>32</v>
       </c>
       <c r="T9" t="s">
+        <v>32</v>
+      </c>
+      <c r="U9" t="s">
+        <v>32</v>
+      </c>
+      <c r="V9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>127</v>
       </c>
       <c r="F10" t="s">
-        <v>90</v>
-      </c>
-      <c r="G10" t="s">
-        <v>91</v>
+        <v>32</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3.0</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>128</v>
       </c>
       <c r="I10" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="J10" t="s">
         <v>32</v>
@@ -2347,49 +2491,55 @@
       <c r="O10" t="s">
         <v>32</v>
       </c>
-      <c r="P10" t="b">
+      <c r="P10" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R10" t="b">
         <v>0</v>
       </c>
-      <c r="Q10" t="s">
-        <v>32</v>
-      </c>
-      <c r="R10" t="s">
-        <v>32</v>
-      </c>
       <c r="S10" t="s">
         <v>32</v>
       </c>
       <c r="T10" t="s">
+        <v>32</v>
+      </c>
+      <c r="U10" t="s">
+        <v>32</v>
+      </c>
+      <c r="V10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="C11" t="s">
         <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>120</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="F11" t="s">
-        <v>90</v>
-      </c>
-      <c r="G11" t="s">
-        <v>68</v>
+        <v>32</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.0</v>
       </c>
       <c r="H11" t="s">
-        <v>32</v>
+        <v>131</v>
       </c>
       <c r="I11" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="J11" t="s">
         <v>32</v>
@@ -2409,49 +2559,55 @@
       <c r="O11" t="s">
         <v>32</v>
       </c>
-      <c r="P11" t="b">
+      <c r="P11" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>32</v>
+      </c>
+      <c r="R11" t="b">
         <v>0</v>
       </c>
-      <c r="Q11" t="s">
-        <v>32</v>
-      </c>
-      <c r="R11" t="s">
-        <v>32</v>
-      </c>
       <c r="S11" t="s">
         <v>32</v>
       </c>
       <c r="T11" t="s">
+        <v>32</v>
+      </c>
+      <c r="U11" t="s">
+        <v>32</v>
+      </c>
+      <c r="V11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>89</v>
+        <v>134</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>135</v>
       </c>
       <c r="F12" t="s">
-        <v>90</v>
-      </c>
-      <c r="G12" t="s">
-        <v>69</v>
+        <v>32</v>
+      </c>
+      <c r="G12" t="n">
+        <v>3.0</v>
       </c>
       <c r="H12" t="s">
-        <v>32</v>
+        <v>136</v>
       </c>
       <c r="I12" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="J12" t="s">
         <v>32</v>
@@ -2471,49 +2627,55 @@
       <c r="O12" t="s">
         <v>32</v>
       </c>
-      <c r="P12" t="b">
+      <c r="P12" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>32</v>
+      </c>
+      <c r="R12" t="b">
         <v>0</v>
       </c>
-      <c r="Q12" t="s">
-        <v>32</v>
-      </c>
-      <c r="R12" t="s">
-        <v>32</v>
-      </c>
       <c r="S12" t="s">
         <v>32</v>
       </c>
       <c r="T12" t="s">
+        <v>32</v>
+      </c>
+      <c r="U12" t="s">
+        <v>32</v>
+      </c>
+      <c r="V12" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>117</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>111</v>
       </c>
       <c r="F13" t="s">
-        <v>90</v>
-      </c>
-      <c r="G13" t="s">
-        <v>70</v>
+        <v>32</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3.0</v>
       </c>
       <c r="H13" t="s">
-        <v>32</v>
+        <v>139</v>
       </c>
       <c r="I13" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="J13" t="s">
         <v>32</v>
@@ -2533,49 +2695,55 @@
       <c r="O13" t="s">
         <v>32</v>
       </c>
-      <c r="P13" t="b">
+      <c r="P13" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>32</v>
+      </c>
+      <c r="R13" t="b">
         <v>0</v>
       </c>
-      <c r="Q13" t="s">
-        <v>32</v>
-      </c>
-      <c r="R13" t="s">
-        <v>32</v>
-      </c>
       <c r="S13" t="s">
         <v>32</v>
       </c>
       <c r="T13" t="s">
+        <v>32</v>
+      </c>
+      <c r="U13" t="s">
+        <v>32</v>
+      </c>
+      <c r="V13" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="B14" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="C14" t="s">
         <v>34</v>
       </c>
       <c r="D14" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" t="s">
         <v>106</v>
       </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
       <c r="F14" t="s">
-        <v>90</v>
-      </c>
-      <c r="G14" t="s">
-        <v>71</v>
+        <v>32</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3.0</v>
       </c>
       <c r="H14" t="s">
-        <v>32</v>
+        <v>142</v>
       </c>
       <c r="I14" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="J14" t="s">
         <v>32</v>
@@ -2595,49 +2763,55 @@
       <c r="O14" t="s">
         <v>32</v>
       </c>
-      <c r="P14" t="b">
+      <c r="P14" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>32</v>
+      </c>
+      <c r="R14" t="b">
         <v>0</v>
       </c>
-      <c r="Q14" t="s">
-        <v>32</v>
-      </c>
-      <c r="R14" t="s">
-        <v>32</v>
-      </c>
       <c r="S14" t="s">
         <v>32</v>
       </c>
       <c r="T14" t="s">
+        <v>32</v>
+      </c>
+      <c r="U14" t="s">
+        <v>32</v>
+      </c>
+      <c r="V14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="B15" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="C15" t="s">
         <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="F15" t="s">
-        <v>90</v>
-      </c>
-      <c r="G15" t="s">
-        <v>72</v>
+        <v>32</v>
+      </c>
+      <c r="G15" t="n">
+        <v>3.0</v>
       </c>
       <c r="H15" t="s">
-        <v>32</v>
+        <v>145</v>
       </c>
       <c r="I15" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="J15" t="s">
         <v>32</v>
@@ -2657,49 +2831,55 @@
       <c r="O15" t="s">
         <v>32</v>
       </c>
-      <c r="P15" t="b">
+      <c r="P15" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>32</v>
+      </c>
+      <c r="R15" t="b">
         <v>0</v>
       </c>
-      <c r="Q15" t="s">
-        <v>32</v>
-      </c>
-      <c r="R15" t="s">
-        <v>32</v>
-      </c>
       <c r="S15" t="s">
         <v>32</v>
       </c>
       <c r="T15" t="s">
+        <v>32</v>
+      </c>
+      <c r="U15" t="s">
+        <v>32</v>
+      </c>
+      <c r="V15" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="C16" t="s">
         <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>148</v>
       </c>
       <c r="F16" t="s">
-        <v>90</v>
-      </c>
-      <c r="G16" t="s">
-        <v>108</v>
+        <v>32</v>
+      </c>
+      <c r="G16" t="n">
+        <v>3.0</v>
       </c>
       <c r="H16" t="s">
-        <v>32</v>
+        <v>149</v>
       </c>
       <c r="I16" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="J16" t="s">
         <v>32</v>
@@ -2719,49 +2899,55 @@
       <c r="O16" t="s">
         <v>32</v>
       </c>
-      <c r="P16" t="b">
+      <c r="P16" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>32</v>
+      </c>
+      <c r="R16" t="b">
         <v>0</v>
       </c>
-      <c r="Q16" t="s">
-        <v>32</v>
-      </c>
-      <c r="R16" t="s">
-        <v>32</v>
-      </c>
       <c r="S16" t="s">
         <v>32</v>
       </c>
       <c r="T16" t="s">
+        <v>32</v>
+      </c>
+      <c r="U16" t="s">
+        <v>32</v>
+      </c>
+      <c r="V16" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="B17" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="C17" t="s">
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>133</v>
+        <v>75</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="F17" t="s">
-        <v>90</v>
-      </c>
-      <c r="G17" t="s">
-        <v>112</v>
+        <v>32</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.0</v>
       </c>
       <c r="H17" t="s">
-        <v>32</v>
+        <v>152</v>
       </c>
       <c r="I17" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="J17" t="s">
         <v>32</v>
@@ -2781,49 +2967,55 @@
       <c r="O17" t="s">
         <v>32</v>
       </c>
-      <c r="P17" t="b">
+      <c r="P17" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>32</v>
+      </c>
+      <c r="R17" t="b">
         <v>0</v>
       </c>
-      <c r="Q17" t="s">
-        <v>32</v>
-      </c>
-      <c r="R17" t="s">
-        <v>32</v>
-      </c>
       <c r="S17" t="s">
         <v>32</v>
       </c>
       <c r="T17" t="s">
+        <v>32</v>
+      </c>
+      <c r="U17" t="s">
+        <v>32</v>
+      </c>
+      <c r="V17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="B18" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C18" t="s">
         <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>155</v>
       </c>
       <c r="F18" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18" t="s">
-        <v>77</v>
+        <v>32</v>
+      </c>
+      <c r="G18" t="n">
+        <v>2.0</v>
       </c>
       <c r="H18" t="s">
-        <v>32</v>
+        <v>156</v>
       </c>
       <c r="I18" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="J18" t="s">
         <v>32</v>
@@ -2843,49 +3035,55 @@
       <c r="O18" t="s">
         <v>32</v>
       </c>
-      <c r="P18" t="b">
+      <c r="P18" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>32</v>
+      </c>
+      <c r="R18" t="b">
         <v>0</v>
       </c>
-      <c r="Q18" t="s">
-        <v>32</v>
-      </c>
-      <c r="R18" t="s">
-        <v>32</v>
-      </c>
       <c r="S18" t="s">
         <v>32</v>
       </c>
       <c r="T18" t="s">
+        <v>32</v>
+      </c>
+      <c r="U18" t="s">
+        <v>32</v>
+      </c>
+      <c r="V18" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="B19" t="s">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="C19" t="s">
         <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>117</v>
+        <v>159</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>160</v>
       </c>
       <c r="F19" t="s">
-        <v>90</v>
-      </c>
-      <c r="G19" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.0</v>
       </c>
       <c r="H19" t="s">
-        <v>32</v>
+        <v>161</v>
       </c>
       <c r="I19" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="J19" t="s">
         <v>32</v>
@@ -2905,19 +3103,25 @@
       <c r="O19" t="s">
         <v>32</v>
       </c>
-      <c r="P19" t="b">
+      <c r="P19" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>32</v>
+      </c>
+      <c r="R19" t="b">
         <v>0</v>
       </c>
-      <c r="Q19" t="s">
-        <v>32</v>
-      </c>
-      <c r="R19" t="s">
-        <v>32</v>
-      </c>
       <c r="S19" t="s">
         <v>32</v>
       </c>
       <c r="T19" t="s">
+        <v>32</v>
+      </c>
+      <c r="U19" t="s">
+        <v>32</v>
+      </c>
+      <c r="V19" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2937,13 +3141,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="12.203125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="19.91015625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="11.86328125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2971,7 +3175,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>43</v>
@@ -2994,26 +3198,16 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3"/>
+      <c r="C3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" t="s">
-        <v>32</v>
-      </c>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
     </row>
   </sheetData>
   <sheetProtection password="D4D4" sheet="true" scenarios="true" objects="true"/>
@@ -3035,13 +3229,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="11.94140625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="13.6171875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="13.6171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.23828125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="11.86328125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3069,7 +3263,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>43</v>
@@ -3088,6 +3282,357 @@
       </c>
       <c r="G2" s="1" t="s">
         <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection password="D4D4" sheet="true" scenarios="true" objects="true"/>
+  <mergeCells>
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="11.86328125" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
conf scheduling: add room and content view
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView activeTab="2"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" r:id="rId3" sheetId="1"/>
@@ -11,15 +11,17 @@
     <sheet name="Rooms" r:id="rId5" sheetId="3"/>
     <sheet name="Speakers" r:id="rId6" sheetId="4"/>
     <sheet name="Talks" r:id="rId7" sheetId="5"/>
-    <sheet name="Theme view" r:id="rId8" sheetId="6"/>
-    <sheet name="Sector view" r:id="rId9" sheetId="7"/>
-    <sheet name="Speaker view" r:id="rId10" sheetId="8"/>
+    <sheet name="Room view" r:id="rId8" sheetId="6"/>
+    <sheet name="Speaker view" r:id="rId9" sheetId="7"/>
+    <sheet name="Theme view" r:id="rId10" sheetId="8"/>
+    <sheet name="Sector view" r:id="rId11" sheetId="9"/>
+    <sheet name="Content view" r:id="rId12" sheetId="10"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="167">
   <si>
     <t>Conference name</t>
   </si>
@@ -507,13 +509,19 @@
     <t>VertX</t>
   </si>
   <si>
+    <t>Speaker</t>
+  </si>
+  <si>
     <t>Theme tag</t>
   </si>
   <si>
     <t>Sector tag</t>
   </si>
   <si>
-    <t>Speaker</t>
+    <t>Content tag</t>
+  </si>
+  <si>
+    <t>(1) S06</t>
   </si>
 </sst>
 </file>
@@ -751,6 +759,94 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="11.78515625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="11.86328125" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3"/>
+      <c r="C3" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+    </row>
+  </sheetData>
+  <sheetProtection password="D4D4" sheet="true" scenarios="true" objects="true"/>
+  <mergeCells>
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
@@ -3135,7 +3231,548 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="6.44921875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="11.86328125" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection password="D4D4" sheet="true" scenarios="true" objects="true"/>
+  <mergeCells>
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="11.86328125" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection password="D4D4" sheet="true" scenarios="true" objects="true"/>
+  <mergeCells>
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -3175,7 +3812,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>43</v>
@@ -3218,12 +3855,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -3263,7 +3900,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>43</v>
@@ -3282,357 +3919,6 @@
       </c>
       <c r="G2" s="1" t="s">
         <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection password="D4D4" sheet="true" scenarios="true" objects="true"/>
-  <mergeCells>
-    <mergeCell ref="B1:G1"/>
-  </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="11.86328125" customWidth="true" bestFit="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
conf scheduling: add constraint "Content audience level flow violation" (thanks Stephan)
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
@@ -20,8 +20,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+    <author>OptaPlanner</author>
+  </authors>
+  <commentList>
+    <comment ref="C3" authorId="1">
+      <text>
+        <t>Speaker unavailable timeslots (S06): -1hard</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+    <author>OptaPlanner</author>
+  </authors>
+  <commentList>
+    <comment ref="C3" authorId="1">
+      <text>
+        <t>Speaker unavailable timeslots (S06): -1hard</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="169">
   <si>
     <t>Conference name</t>
   </si>
@@ -48,6 +80,12 @@
   </si>
   <si>
     <t>Soft penalty per common sector of 2 talks that have an overlapping timeslot</t>
+  </si>
+  <si>
+    <t>Content audience level flow violation</t>
+  </si>
+  <si>
+    <t>Soft penalty per common content of 2 talks with a different audience level for which the easier talk isn't scheduled earlier than the other talk.</t>
   </si>
   <si>
     <t>Language diversity</t>
@@ -597,8 +635,48 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
@@ -608,9 +686,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="29.5" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="35.140625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.80859375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="70.88671875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="130.52734375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -696,12 +774,12 @@
         <v>10.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" t="n">
         <v>10.0</v>
@@ -712,13 +790,13 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" t="n">
         <v>10.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12">
@@ -740,12 +818,12 @@
         <v>10.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B14" t="n">
         <v>10.0</v>
@@ -754,13 +832,25 @@
         <v>20</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -781,57 +871,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B3"/>
       <c r="C3" s="4" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -839,16 +929,17 @@
       <c r="G3"/>
     </row>
   </sheetData>
-  <sheetProtection password="D4D4" sheet="true" scenarios="true" objects="true"/>
   <mergeCells>
     <mergeCell ref="B1:G1"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -867,130 +958,131 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1012,184 +1104,184 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1197,11 +1289,12 @@
     <mergeCell ref="C1:H1"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1230,660 +1323,660 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1891,11 +1984,12 @@
     <mergeCell ref="J1:O1"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1931,1303 +2025,1304 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="U1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G2" t="n">
         <v>2.0</v>
       </c>
       <c r="H2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R2" t="b">
         <v>0</v>
       </c>
       <c r="S2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="V2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G3" t="n">
         <v>1.0</v>
       </c>
       <c r="H3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R3" t="b">
         <v>0</v>
       </c>
       <c r="S3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="V3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G4" t="n">
         <v>3.0</v>
       </c>
       <c r="H4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R4" t="b">
         <v>0</v>
       </c>
       <c r="S4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="V4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G5" t="n">
         <v>2.0</v>
       </c>
       <c r="H5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R5" t="b">
         <v>0</v>
       </c>
       <c r="S5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="V5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G6" t="n">
         <v>3.0</v>
       </c>
       <c r="H6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R6" t="b">
         <v>0</v>
       </c>
       <c r="S6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="V6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G7" t="n">
         <v>1.0</v>
       </c>
       <c r="H7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R7" t="b">
         <v>0</v>
       </c>
       <c r="S7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="V7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G8" t="n">
         <v>1.0</v>
       </c>
       <c r="H8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="I8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R8" s="3" t="b">
         <v>1</v>
       </c>
       <c r="S8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="T8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="U8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="V8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E9" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G9" t="n">
         <v>2.0</v>
       </c>
       <c r="H9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R9" t="b">
         <v>0</v>
       </c>
       <c r="S9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="V9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E10" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G10" t="n">
         <v>3.0</v>
       </c>
       <c r="H10" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="I10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R10" t="b">
         <v>0</v>
       </c>
       <c r="S10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="V10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G11" t="n">
         <v>1.0</v>
       </c>
       <c r="H11" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I11" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R11" t="b">
         <v>0</v>
       </c>
       <c r="S11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="V11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B12" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G12" t="n">
         <v>3.0</v>
       </c>
       <c r="H12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I12" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R12" t="b">
         <v>0</v>
       </c>
       <c r="S12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="V12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B13" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G13" t="n">
         <v>3.0</v>
       </c>
       <c r="H13" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="I13" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R13" t="b">
         <v>0</v>
       </c>
       <c r="S13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="V13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B14" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E14" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G14" t="n">
         <v>3.0</v>
       </c>
       <c r="H14" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I14" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R14" t="b">
         <v>0</v>
       </c>
       <c r="S14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="V14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B15" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E15" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G15" t="n">
         <v>3.0</v>
       </c>
       <c r="H15" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I15" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R15" t="b">
         <v>0</v>
       </c>
       <c r="S15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="V15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B16" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E16" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G16" t="n">
         <v>3.0</v>
       </c>
       <c r="H16" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I16" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R16" t="b">
         <v>0</v>
       </c>
       <c r="S16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="V16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B17" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E17" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G17" t="n">
         <v>1.0</v>
       </c>
       <c r="H17" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I17" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R17" t="b">
         <v>0</v>
       </c>
       <c r="S17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="V17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B18" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E18" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G18" t="n">
         <v>2.0</v>
       </c>
       <c r="H18" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="I18" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R18" t="b">
         <v>0</v>
       </c>
       <c r="S18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="V18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B19" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E19" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F19" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G19" t="n">
         <v>1.0</v>
       </c>
       <c r="H19" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="I19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R19" t="b">
         <v>0</v>
       </c>
       <c r="S19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="V19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3248,176 +3343,176 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="D4D4" sheet="true" scenarios="true" objects="true"/>
   <mergeCells>
     <mergeCell ref="B1:G1"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3438,337 +3533,337 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="D4D4" sheet="true" scenarios="true" objects="true"/>
   <mergeCells>
     <mergeCell ref="B1:G1"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3789,57 +3884,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B3"/>
       <c r="C3" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -3847,16 +3942,17 @@
       <c r="G3"/>
     </row>
   </sheetData>
-  <sheetProtection password="D4D4" sheet="true" scenarios="true" objects="true"/>
   <mergeCells>
     <mergeCell ref="B1:G1"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3877,55 +3973,55 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="D4D4" sheet="true" scenarios="true" objects="true"/>
   <mergeCells>
     <mergeCell ref="B1:G1"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
conf scheduling: Pinned talks only need to be set in the talks sheet. Room view shows solutions
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
@@ -11,11 +11,11 @@
     <sheet name="Rooms" r:id="rId5" sheetId="3"/>
     <sheet name="Speakers" r:id="rId6" sheetId="4"/>
     <sheet name="Talks" r:id="rId7" sheetId="5"/>
-    <sheet name="Room view" r:id="rId8" sheetId="6"/>
-    <sheet name="Speaker view" r:id="rId9" sheetId="7"/>
-    <sheet name="Theme view" r:id="rId10" sheetId="8"/>
-    <sheet name="Sector view" r:id="rId11" sheetId="9"/>
-    <sheet name="Content view" r:id="rId12" sheetId="10"/>
+    <sheet name="Rooms view" r:id="rId8" sheetId="6"/>
+    <sheet name="Speakers view" r:id="rId9" sheetId="7"/>
+    <sheet name="Theme tracks view" r:id="rId10" sheetId="8"/>
+    <sheet name="Sectors view" r:id="rId11" sheetId="9"/>
+    <sheet name="Contents view" r:id="rId12" sheetId="10"/>
   </sheets>
 </workbook>
 </file>
@@ -70,10 +70,10 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Theme conflict</t>
-  </si>
-  <si>
-    <t>Soft penalty per common theme of 2 talks that have an overlapping timeslot</t>
+    <t>Theme track conflict</t>
+  </si>
+  <si>
+    <t>Soft penalty per common theme track of 2 talks that have an overlapping timeslot</t>
   </si>
   <si>
     <t>Sector conflict</t>
@@ -214,207 +214,207 @@
     <t>Large, Recorded</t>
   </si>
   <si>
+    <t>R 2</t>
+  </si>
+  <si>
+    <t>R 3</t>
+  </si>
+  <si>
+    <t>Recorded</t>
+  </si>
+  <si>
+    <t>R 4</t>
+  </si>
+  <si>
+    <t>R 5</t>
+  </si>
+  <si>
+    <t>Lab_room, Large, Recorded</t>
+  </si>
+  <si>
+    <t>Required timeslot tags</t>
+  </si>
+  <si>
+    <t>Preferred timeslot tags</t>
+  </si>
+  <si>
+    <t>Prohibited timeslot tags</t>
+  </si>
+  <si>
+    <t>Undesired timeslot tags</t>
+  </si>
+  <si>
+    <t>Required room tags</t>
+  </si>
+  <si>
+    <t>Preferred room tags</t>
+  </si>
+  <si>
+    <t>Prohibited room tags</t>
+  </si>
+  <si>
+    <t>Undesired room tags</t>
+  </si>
+  <si>
+    <t>Amy Cole</t>
+  </si>
+  <si>
+    <t>Beth Fox</t>
+  </si>
+  <si>
+    <t>Chad Green</t>
+  </si>
+  <si>
+    <t>Dan Jones</t>
+  </si>
+  <si>
+    <t>Elsa King</t>
+  </si>
+  <si>
+    <t>Flo Li</t>
+  </si>
+  <si>
+    <t>Gus Poe</t>
+  </si>
+  <si>
+    <t>Hugo Rye</t>
+  </si>
+  <si>
+    <t>Ivy Smith</t>
+  </si>
+  <si>
+    <t>Jay Watt</t>
+  </si>
+  <si>
+    <t>Amy Fox</t>
+  </si>
+  <si>
+    <t>Beth Green</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Speakers</t>
+  </si>
+  <si>
+    <t>Theme track tags</t>
+  </si>
+  <si>
+    <t>Sector tags</t>
+  </si>
+  <si>
+    <t>Audience level</t>
+  </si>
+  <si>
+    <t>Content tags</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Pinned by user</t>
+  </si>
+  <si>
+    <t>Timeslot day</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>S00</t>
+  </si>
+  <si>
+    <t>Hands on real-time OpenShift</t>
+  </si>
+  <si>
+    <t>Cloud</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>OpenShift, Kubernetes</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>Lab_room</t>
+  </si>
+  <si>
+    <t>S01</t>
+  </si>
+  <si>
+    <t>Advanced containerized WildFly</t>
+  </si>
+  <si>
+    <t>Big Data</t>
+  </si>
+  <si>
+    <t>WildFly</t>
+  </si>
+  <si>
+    <t>S02</t>
+  </si>
+  <si>
+    <t>Learn virtualized Spring</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>S03</t>
+  </si>
+  <si>
+    <t>Intro to serverless Drools</t>
+  </si>
+  <si>
+    <t>Culture</t>
+  </si>
+  <si>
+    <t>Drools</t>
+  </si>
+  <si>
+    <t>S04</t>
+  </si>
+  <si>
+    <t>Discover AI-driven OptaPlanner</t>
+  </si>
+  <si>
+    <t>Elsa King, Flo Li</t>
+  </si>
+  <si>
+    <t>IoT</t>
+  </si>
+  <si>
+    <t>OptaPlanner</t>
+  </si>
+  <si>
+    <t>S05</t>
+  </si>
+  <si>
+    <t>Mastering machine learning jBPM</t>
+  </si>
+  <si>
+    <t>Gus Poe, Hugo Rye</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>jBPM</t>
+  </si>
+  <si>
     <t>S06</t>
   </si>
   <si>
-    <t>R 2</t>
-  </si>
-  <si>
-    <t>R 3</t>
-  </si>
-  <si>
-    <t>Recorded</t>
-  </si>
-  <si>
-    <t>R 4</t>
-  </si>
-  <si>
-    <t>R 5</t>
-  </si>
-  <si>
-    <t>Lab_room, Large, Recorded</t>
-  </si>
-  <si>
-    <t>Required timeslot tags</t>
-  </si>
-  <si>
-    <t>Preferred timeslot tags</t>
-  </si>
-  <si>
-    <t>Prohibited timeslot tags</t>
-  </si>
-  <si>
-    <t>Undesired timeslot tags</t>
-  </si>
-  <si>
-    <t>Required room tags</t>
-  </si>
-  <si>
-    <t>Preferred room tags</t>
-  </si>
-  <si>
-    <t>Prohibited room tags</t>
-  </si>
-  <si>
-    <t>Undesired room tags</t>
-  </si>
-  <si>
-    <t>Amy Cole</t>
-  </si>
-  <si>
-    <t>Beth Fox</t>
-  </si>
-  <si>
-    <t>Chad Green</t>
-  </si>
-  <si>
-    <t>Dan Jones</t>
-  </si>
-  <si>
-    <t>Elsa King</t>
-  </si>
-  <si>
-    <t>Flo Li</t>
-  </si>
-  <si>
-    <t>Gus Poe</t>
-  </si>
-  <si>
-    <t>Hugo Rye</t>
-  </si>
-  <si>
-    <t>Ivy Smith</t>
-  </si>
-  <si>
-    <t>Jay Watt</t>
-  </si>
-  <si>
-    <t>Amy Fox</t>
-  </si>
-  <si>
-    <t>Beth Green</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Speakers</t>
-  </si>
-  <si>
-    <t>Theme tags</t>
-  </si>
-  <si>
-    <t>Sector tags</t>
-  </si>
-  <si>
-    <t>Audience level</t>
-  </si>
-  <si>
-    <t>Content tags</t>
-  </si>
-  <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>Pinned by user</t>
-  </si>
-  <si>
-    <t>Timeslot day</t>
-  </si>
-  <si>
-    <t>Room</t>
-  </si>
-  <si>
-    <t>S00</t>
-  </si>
-  <si>
-    <t>Hands on real-time OpenShift</t>
-  </si>
-  <si>
-    <t>Cloud</t>
-  </si>
-  <si>
-    <t>Government</t>
-  </si>
-  <si>
-    <t>OpenShift, Kubernetes</t>
-  </si>
-  <si>
-    <t>en</t>
-  </si>
-  <si>
-    <t>Lab_room</t>
-  </si>
-  <si>
-    <t>S01</t>
-  </si>
-  <si>
-    <t>Advanced containerized WildFly</t>
-  </si>
-  <si>
-    <t>Big Data</t>
-  </si>
-  <si>
-    <t>WildFly</t>
-  </si>
-  <si>
-    <t>S02</t>
-  </si>
-  <si>
-    <t>Learn virtualized Spring</t>
-  </si>
-  <si>
-    <t>Mobile</t>
-  </si>
-  <si>
-    <t>Spring</t>
-  </si>
-  <si>
-    <t>S03</t>
-  </si>
-  <si>
-    <t>Intro to serverless Drools</t>
-  </si>
-  <si>
-    <t>Culture</t>
-  </si>
-  <si>
-    <t>Drools</t>
-  </si>
-  <si>
-    <t>S04</t>
-  </si>
-  <si>
-    <t>Discover AI-driven OptaPlanner</t>
-  </si>
-  <si>
-    <t>Elsa King, Flo Li</t>
-  </si>
-  <si>
-    <t>IoT</t>
-  </si>
-  <si>
-    <t>OptaPlanner</t>
-  </si>
-  <si>
-    <t>S05</t>
-  </si>
-  <si>
-    <t>Mastering machine learning jBPM</t>
-  </si>
-  <si>
-    <t>Gus Poe, Hugo Rye</t>
-  </si>
-  <si>
-    <t>Security</t>
-  </si>
-  <si>
-    <t>jBPM</t>
-  </si>
-  <si>
     <t>Tuning IOT-driven Camel</t>
   </si>
   <si>
@@ -550,7 +550,7 @@
     <t>Speaker</t>
   </si>
   <si>
-    <t>Theme tag</t>
+    <t>Theme track tag</t>
   </si>
   <si>
     <t>Sector tag</t>
@@ -1164,8 +1164,8 @@
       <c r="C3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>53</v>
+      <c r="D3" t="s">
+        <v>34</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -1208,10 +1208,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
         <v>55</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>34</v>
@@ -1234,10 +1234,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>34</v>
@@ -1260,10 +1260,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
         <v>58</v>
-      </c>
-      <c r="B7" t="s">
-        <v>59</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
@@ -1373,28 +1373,28 @@
         <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>45</v>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
@@ -1529,7 +1529,7 @@
         <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H5" t="s">
         <v>34</v>
@@ -1558,7 +1558,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
         <v>34</v>
@@ -1605,7 +1605,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>34</v>
@@ -1652,7 +1652,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
@@ -1699,7 +1699,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
         <v>34</v>
@@ -1717,7 +1717,7 @@
         <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H9" t="s">
         <v>34</v>
@@ -1746,7 +1746,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
@@ -1793,7 +1793,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
         <v>34</v>
@@ -1823,7 +1823,7 @@
         <v>34</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>34</v>
@@ -1840,7 +1840,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
         <v>34</v>
@@ -1858,7 +1858,7 @@
         <v>34</v>
       </c>
       <c r="G12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H12" t="s">
         <v>34</v>
@@ -1887,7 +1887,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
         <v>34</v>
@@ -1934,7 +1934,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -2025,61 +2025,61 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>26</v>
@@ -2088,51 +2088,51 @@
         <v>27</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" t="s">
         <v>91</v>
-      </c>
-      <c r="B2" t="s">
-        <v>92</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" t="s">
         <v>93</v>
-      </c>
-      <c r="F2" t="s">
-        <v>94</v>
       </c>
       <c r="G2" t="n">
         <v>2.0</v>
       </c>
       <c r="H2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" t="s">
         <v>95</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" t="s">
         <v>96</v>
-      </c>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" t="s">
-        <v>34</v>
-      </c>
-      <c r="N2" t="s">
-        <v>97</v>
       </c>
       <c r="O2" t="s">
         <v>34</v>
@@ -2161,19 +2161,19 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
         <v>98</v>
-      </c>
-      <c r="B3" t="s">
-        <v>99</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F3" t="s">
         <v>34</v>
@@ -2182,25 +2182,25 @@
         <v>1.0</v>
       </c>
       <c r="H3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" t="s">
         <v>96</v>
-      </c>
-      <c r="J3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3" t="s">
-        <v>97</v>
       </c>
       <c r="O3" t="s">
         <v>34</v>
@@ -2229,19 +2229,19 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" t="s">
         <v>102</v>
-      </c>
-      <c r="B4" t="s">
-        <v>103</v>
       </c>
       <c r="C4" t="s">
         <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F4" t="s">
         <v>34</v>
@@ -2250,10 +2250,10 @@
         <v>3.0</v>
       </c>
       <c r="H4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J4" t="s">
         <v>34</v>
@@ -2297,19 +2297,19 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
         <v>106</v>
-      </c>
-      <c r="B5" t="s">
-        <v>107</v>
       </c>
       <c r="C5" t="s">
         <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F5" t="s">
         <v>34</v>
@@ -2318,10 +2318,10 @@
         <v>2.0</v>
       </c>
       <c r="H5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J5" t="s">
         <v>34</v>
@@ -2365,19 +2365,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" t="s">
         <v>110</v>
-      </c>
-      <c r="B6" t="s">
-        <v>111</v>
       </c>
       <c r="C6" t="s">
         <v>36</v>
       </c>
       <c r="D6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" t="s">
         <v>112</v>
-      </c>
-      <c r="E6" t="s">
-        <v>113</v>
       </c>
       <c r="F6" t="s">
         <v>34</v>
@@ -2386,10 +2386,10 @@
         <v>3.0</v>
       </c>
       <c r="H6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J6" t="s">
         <v>34</v>
@@ -2433,19 +2433,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" t="s">
         <v>115</v>
-      </c>
-      <c r="B7" t="s">
-        <v>116</v>
       </c>
       <c r="C7" t="s">
         <v>36</v>
       </c>
       <c r="D7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" t="s">
         <v>117</v>
-      </c>
-      <c r="E7" t="s">
-        <v>118</v>
       </c>
       <c r="F7" t="s">
         <v>34</v>
@@ -2454,10 +2454,10 @@
         <v>1.0</v>
       </c>
       <c r="H7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J7" t="s">
         <v>34</v>
@@ -2501,7 +2501,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
         <v>120</v>
@@ -2510,7 +2510,7 @@
         <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E8" t="s">
         <v>121</v>
@@ -2525,7 +2525,7 @@
         <v>122</v>
       </c>
       <c r="I8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J8" t="s">
         <v>34</v>
@@ -2578,10 +2578,10 @@
         <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F9" t="s">
         <v>34</v>
@@ -2593,7 +2593,7 @@
         <v>125</v>
       </c>
       <c r="I9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J9" t="s">
         <v>34</v>
@@ -2661,7 +2661,7 @@
         <v>130</v>
       </c>
       <c r="I10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J10" t="s">
         <v>34</v>
@@ -2714,7 +2714,7 @@
         <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
         <v>121</v>
@@ -2729,7 +2729,7 @@
         <v>133</v>
       </c>
       <c r="I11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J11" t="s">
         <v>34</v>
@@ -2797,7 +2797,7 @@
         <v>138</v>
       </c>
       <c r="I12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J12" t="s">
         <v>34</v>
@@ -2850,10 +2850,10 @@
         <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F13" t="s">
         <v>34</v>
@@ -2865,7 +2865,7 @@
         <v>141</v>
       </c>
       <c r="I13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J13" t="s">
         <v>34</v>
@@ -2918,10 +2918,10 @@
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F14" t="s">
         <v>34</v>
@@ -2933,7 +2933,7 @@
         <v>144</v>
       </c>
       <c r="I14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J14" t="s">
         <v>34</v>
@@ -2986,10 +2986,10 @@
         <v>36</v>
       </c>
       <c r="D15" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" t="s">
         <v>117</v>
-      </c>
-      <c r="E15" t="s">
-        <v>118</v>
       </c>
       <c r="F15" t="s">
         <v>34</v>
@@ -3001,7 +3001,7 @@
         <v>147</v>
       </c>
       <c r="I15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J15" t="s">
         <v>34</v>
@@ -3054,7 +3054,7 @@
         <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E16" t="s">
         <v>150</v>
@@ -3069,7 +3069,7 @@
         <v>151</v>
       </c>
       <c r="I16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J16" t="s">
         <v>34</v>
@@ -3122,10 +3122,10 @@
         <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F17" t="s">
         <v>34</v>
@@ -3137,7 +3137,7 @@
         <v>154</v>
       </c>
       <c r="I17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J17" t="s">
         <v>34</v>
@@ -3205,7 +3205,7 @@
         <v>158</v>
       </c>
       <c r="I18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J18" t="s">
         <v>34</v>
@@ -3264,7 +3264,7 @@
         <v>162</v>
       </c>
       <c r="F19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G19" t="n">
         <v>1.0</v>
@@ -3273,7 +3273,7 @@
         <v>163</v>
       </c>
       <c r="I19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J19" t="s">
         <v>34</v>
@@ -3366,7 +3366,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>45</v>
@@ -3395,7 +3395,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
       <c r="D3" t="s">
         <v>34</v>
@@ -3412,7 +3412,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>34</v>
@@ -3435,7 +3435,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>34</v>
@@ -3458,7 +3458,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>34</v>
@@ -3481,7 +3481,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
         <v>34</v>
@@ -3579,7 +3579,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -3602,7 +3602,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -3625,7 +3625,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
@@ -3648,7 +3648,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
         <v>34</v>
@@ -3671,7 +3671,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>34</v>
@@ -3694,7 +3694,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
@@ -3717,7 +3717,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
         <v>34</v>
@@ -3740,7 +3740,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
@@ -3763,13 +3763,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>34</v>
@@ -3786,7 +3786,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
         <v>34</v>
@@ -3809,7 +3809,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
         <v>34</v>
@@ -3832,7 +3832,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -3934,7 +3934,7 @@
       </c>
       <c r="B3"/>
       <c r="C3" s="4" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>

</xml_diff>

<commit_message>
Add "Audience level diversity" constraint (Mario's request)
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="171">
   <si>
     <t>Conference name</t>
   </si>
@@ -85,7 +85,13 @@
     <t>Content audience level flow violation</t>
   </si>
   <si>
-    <t>Soft penalty per common content of 2 talks with a different audience level for which the easier talk isn't scheduled earlier than the other talk.</t>
+    <t>Soft penalty per common content of 2 talks with a different audience level for which the easier talk isn't scheduled earlier than the other talk</t>
+  </si>
+  <si>
+    <t>Audience level diversity</t>
+  </si>
+  <si>
+    <t>Soft reward per 2 talks that have the same timeslot and a different audience level</t>
   </si>
   <si>
     <t>Language diversity</t>
@@ -688,7 +694,7 @@
   <cols>
     <col min="1" max="1" width="35.140625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.80859375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="130.52734375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="129.94140625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -749,7 +755,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
@@ -785,12 +791,12 @@
         <v>10.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" t="n">
         <v>10.0</v>
@@ -801,13 +807,13 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" t="n">
         <v>10.0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13">
@@ -829,18 +835,29 @@
         <v>10.0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" t="n">
         <v>10.0</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -871,57 +888,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B3"/>
       <c r="C3" s="4" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -958,121 +975,121 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1104,184 +1121,184 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1323,660 +1340,660 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2025,1294 +2042,1294 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="U1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G2" t="n">
         <v>2.0</v>
       </c>
       <c r="H2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="O2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R2" t="b">
         <v>0</v>
       </c>
       <c r="S2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G3" t="n">
         <v>1.0</v>
       </c>
       <c r="H3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="O3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R3" t="b">
         <v>0</v>
       </c>
       <c r="S3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G4" t="n">
         <v>3.0</v>
       </c>
       <c r="H4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R4" t="b">
         <v>0</v>
       </c>
       <c r="S4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G5" t="n">
         <v>2.0</v>
       </c>
       <c r="H5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R5" t="b">
         <v>0</v>
       </c>
       <c r="S5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G6" t="n">
         <v>3.0</v>
       </c>
       <c r="H6" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R6" t="b">
         <v>0</v>
       </c>
       <c r="S6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" t="n">
         <v>1.0</v>
       </c>
       <c r="H7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="I7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R7" t="b">
         <v>0</v>
       </c>
       <c r="S7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G8" t="n">
         <v>1.0</v>
       </c>
       <c r="H8" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="I8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R8" s="3" t="b">
         <v>1</v>
       </c>
       <c r="S8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="T8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="U8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="V8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E9" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" t="n">
         <v>2.0</v>
       </c>
       <c r="H9" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="I9" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R9" t="b">
         <v>0</v>
       </c>
       <c r="S9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B10" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E10" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G10" t="n">
         <v>3.0</v>
       </c>
       <c r="H10" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I10" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R10" t="b">
         <v>0</v>
       </c>
       <c r="S10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B11" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E11" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G11" t="n">
         <v>1.0</v>
       </c>
       <c r="H11" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="I11" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R11" t="b">
         <v>0</v>
       </c>
       <c r="S11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G12" t="n">
         <v>3.0</v>
       </c>
       <c r="H12" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="I12" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R12" t="b">
         <v>0</v>
       </c>
       <c r="S12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B13" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G13" t="n">
         <v>3.0</v>
       </c>
       <c r="H13" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="I13" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R13" t="b">
         <v>0</v>
       </c>
       <c r="S13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B14" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E14" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G14" t="n">
         <v>3.0</v>
       </c>
       <c r="H14" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="I14" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R14" t="b">
         <v>0</v>
       </c>
       <c r="S14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E15" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G15" t="n">
         <v>3.0</v>
       </c>
       <c r="H15" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R15" t="b">
         <v>0</v>
       </c>
       <c r="S15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B16" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E16" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G16" t="n">
         <v>3.0</v>
       </c>
       <c r="H16" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="I16" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R16" t="b">
         <v>0</v>
       </c>
       <c r="S16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B17" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E17" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G17" t="n">
         <v>1.0</v>
       </c>
       <c r="H17" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="I17" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R17" t="b">
         <v>0</v>
       </c>
       <c r="S17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E18" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G18" t="n">
         <v>2.0</v>
       </c>
       <c r="H18" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R18" t="b">
         <v>0</v>
       </c>
       <c r="S18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B19" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E19" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G19" t="n">
         <v>1.0</v>
       </c>
       <c r="H19" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="I19" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R19" t="b">
         <v>0</v>
       </c>
       <c r="S19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -3343,163 +3360,163 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -3533,324 +3550,324 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -3884,57 +3901,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B3"/>
       <c r="C3" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -3973,48 +3990,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
conf scheduling: define all hard constraint names and explain in xlsx
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
@@ -32,7 +32,7 @@
   Ivy Smith
   PINNED BY USER
 Constraint matches:
-  Speaker unavailable timeslots (S06): -1hard</t>
+  Speaker unavailable timeslot (S06): -1hard</t>
       </text>
     </comment>
   </commentList>
@@ -51,7 +51,7 @@
   Ivy Smith
   PINNED BY USER
 Constraint matches:
-  Speaker unavailable timeslots (S06): -1hard</t>
+  Speaker unavailable timeslot (S06): -1hard</t>
       </text>
     </comment>
   </commentList>
@@ -70,7 +70,7 @@
   Ivy Smith
   PINNED BY USER
 Constraint matches:
-  Speaker unavailable timeslots (S06): -1hard</t>
+  Speaker unavailable timeslot (S06): -1hard</t>
       </text>
     </comment>
   </commentList>
@@ -89,7 +89,7 @@
   Ivy Smith
   PINNED BY USER
 Constraint matches:
-  Speaker unavailable timeslots (S06): -1hard</t>
+  Speaker unavailable timeslot (S06): -1hard</t>
       </text>
     </comment>
   </commentList>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="195">
   <si>
     <t>Conference name</t>
   </si>
@@ -178,6 +178,75 @@
   </si>
   <si>
     <t>Talk undesired room tag</t>
+  </si>
+  <si>
+    <t>Talk type of timeslot</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Hard penalty per talk in a timeslot with an other talk type</t>
+  </si>
+  <si>
+    <t>Room unavailable timeslot</t>
+  </si>
+  <si>
+    <t>Hard penalty per talk with an unavailable room at its timeslot</t>
+  </si>
+  <si>
+    <t>Room conflict</t>
+  </si>
+  <si>
+    <t>Hard penalty per pair of talks in the same room in overlapping timeslots</t>
+  </si>
+  <si>
+    <t>Speaker unavailable timeslot</t>
+  </si>
+  <si>
+    <t>Hard penalty per talk with an unavailable speaker at its timeslot</t>
+  </si>
+  <si>
+    <t>Speaker conflict</t>
+  </si>
+  <si>
+    <t>Hard penalty per pair of talks with the same speaker in overlapping timeslots</t>
+  </si>
+  <si>
+    <t>Speaker required timeslot tag</t>
+  </si>
+  <si>
+    <t>Hard penalty per missing required tag in a talk's timeslot</t>
+  </si>
+  <si>
+    <t>Speaker prohibited timeslot tag</t>
+  </si>
+  <si>
+    <t>Hard penalty per prohibited tag in a talk's timeslot</t>
+  </si>
+  <si>
+    <t>Talk required timeslot tag</t>
+  </si>
+  <si>
+    <t>Talk prohibited timeslot tag</t>
+  </si>
+  <si>
+    <t>Speaker required room tag</t>
+  </si>
+  <si>
+    <t>Hard penalty per missing required tag in a talk's room</t>
+  </si>
+  <si>
+    <t>Speaker prohibited room tag</t>
+  </si>
+  <si>
+    <t>Hard penalty per prohibited tag in a talk's room</t>
+  </si>
+  <si>
+    <t>Talk required room tag</t>
+  </si>
+  <si>
+    <t>Talk prohibited room tag</t>
   </si>
   <si>
     <t>Day</t>
@@ -923,6 +992,150 @@
         <v>24</v>
       </c>
     </row>
+    <row r="17"/>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>
@@ -954,71 +1167,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>170</v>
+        <v>193</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>171</v>
+        <v>194</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1051,121 +1264,121 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1197,184 +1410,184 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1416,660 +1629,660 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2118,1294 +2331,1294 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R2" s="2" t="b">
         <v>0</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R3" s="2" t="b">
         <v>0</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>103</v>
+        <v>126</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R4" s="2" t="b">
         <v>0</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R5" s="2" t="b">
         <v>0</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>112</v>
+        <v>135</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>113</v>
+        <v>136</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R6" s="2" t="b">
         <v>0</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="J7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R7" s="2" t="b">
         <v>0</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R8" s="4" t="b">
         <v>1</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>139</v>
+        <v>162</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>145</v>
+        <v>168</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>113</v>
+        <v>136</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G14" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>148</v>
+        <v>171</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G15" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>149</v>
+        <v>172</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>159</v>
+        <v>182</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>161</v>
+        <v>184</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>165</v>
+        <v>188</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3446,163 +3659,163 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" ht="30.0" customHeight="true">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>166</v>
+        <v>189</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" ht="30.0" customHeight="true">
       <c r="A4" s="2" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" ht="30.0" customHeight="true">
       <c r="A5" s="2" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" ht="30.0" customHeight="true">
       <c r="A6" s="2" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" ht="30.0" customHeight="true">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3640,324 +3853,324 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>167</v>
+        <v>190</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" ht="15.0" customHeight="true">
       <c r="A4" s="2" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" ht="15.0" customHeight="true">
       <c r="A5" s="2" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" ht="15.0" customHeight="true">
       <c r="A6" s="2" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="true">
       <c r="A7" s="2" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" ht="15.0" customHeight="true">
       <c r="A8" s="2" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" ht="15.0" customHeight="true">
       <c r="A9" s="2" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" ht="15.0" customHeight="true">
       <c r="A10" s="2" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" ht="15.0" customHeight="true">
       <c r="A11" s="2" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" ht="15.0" customHeight="true">
       <c r="A12" s="2" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" ht="15.0" customHeight="true">
       <c r="A13" s="2" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" ht="15.0" customHeight="true">
       <c r="A14" s="2" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3995,71 +4208,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>168</v>
+        <v>191</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -4097,48 +4310,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>169</v>
+        <v>192</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
conf scheduling: introduce talk type set (for RH Summit)
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="210">
   <si>
     <t>Conference name</t>
   </si>
@@ -304,163 +304,166 @@
     <t>End</t>
   </si>
   <si>
+    <t>Talk types</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Mon 2018-10-01</t>
+  </si>
+  <si>
+    <t>10:15</t>
+  </si>
+  <si>
+    <t>12:15</t>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>Breakout</t>
+  </si>
+  <si>
+    <t>11:30</t>
+  </si>
+  <si>
+    <t>13:00</t>
+  </si>
+  <si>
+    <t>15:00</t>
+  </si>
+  <si>
+    <t>15:30</t>
+  </si>
+  <si>
+    <t>16:15</t>
+  </si>
+  <si>
+    <t>16:30</t>
+  </si>
+  <si>
+    <t>17:15</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>10:15-12:15</t>
+  </si>
+  <si>
+    <t>10:15-11:00</t>
+  </si>
+  <si>
+    <t>11:30-12:15</t>
+  </si>
+  <si>
+    <t>13:00-15:00</t>
+  </si>
+  <si>
+    <t>15:30-16:15</t>
+  </si>
+  <si>
+    <t>16:30-17:15</t>
+  </si>
+  <si>
+    <t>R 1</t>
+  </si>
+  <si>
+    <t>Large, Recorded</t>
+  </si>
+  <si>
+    <t>R 2</t>
+  </si>
+  <si>
+    <t>R 3</t>
+  </si>
+  <si>
+    <t>Recorded</t>
+  </si>
+  <si>
+    <t>R 4</t>
+  </si>
+  <si>
+    <t>R 5</t>
+  </si>
+  <si>
+    <t>Lab_room, Large, Recorded</t>
+  </si>
+  <si>
+    <t>Required timeslot tags</t>
+  </si>
+  <si>
+    <t>Preferred timeslot tags</t>
+  </si>
+  <si>
+    <t>Prohibited timeslot tags</t>
+  </si>
+  <si>
+    <t>Undesired timeslot tags</t>
+  </si>
+  <si>
+    <t>Required room tags</t>
+  </si>
+  <si>
+    <t>Preferred room tags</t>
+  </si>
+  <si>
+    <t>Prohibited room tags</t>
+  </si>
+  <si>
+    <t>Undesired room tags</t>
+  </si>
+  <si>
+    <t>Amy Cole</t>
+  </si>
+  <si>
+    <t>Beth Fox</t>
+  </si>
+  <si>
+    <t>Chad Green</t>
+  </si>
+  <si>
+    <t>Dan Jones</t>
+  </si>
+  <si>
+    <t>Elsa King</t>
+  </si>
+  <si>
+    <t>Flo Li</t>
+  </si>
+  <si>
+    <t>Gus Poe</t>
+  </si>
+  <si>
+    <t>Hugo Rye</t>
+  </si>
+  <si>
+    <t>Ivy Smith</t>
+  </si>
+  <si>
+    <t>Jay Watt</t>
+  </si>
+  <si>
+    <t>Amy Fox</t>
+  </si>
+  <si>
+    <t>Beth Green</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
     <t>Talk type</t>
-  </si>
-  <si>
-    <t>Tags</t>
-  </si>
-  <si>
-    <t>Mon 2018-10-01</t>
-  </si>
-  <si>
-    <t>10:15</t>
-  </si>
-  <si>
-    <t>12:15</t>
-  </si>
-  <si>
-    <t>Lab</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>11:00</t>
-  </si>
-  <si>
-    <t>Breakout</t>
-  </si>
-  <si>
-    <t>11:30</t>
-  </si>
-  <si>
-    <t>13:00</t>
-  </si>
-  <si>
-    <t>15:00</t>
-  </si>
-  <si>
-    <t>15:30</t>
-  </si>
-  <si>
-    <t>16:15</t>
-  </si>
-  <si>
-    <t>16:30</t>
-  </si>
-  <si>
-    <t>17:15</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>10:15-12:15</t>
-  </si>
-  <si>
-    <t>10:15-11:00</t>
-  </si>
-  <si>
-    <t>11:30-12:15</t>
-  </si>
-  <si>
-    <t>13:00-15:00</t>
-  </si>
-  <si>
-    <t>15:30-16:15</t>
-  </si>
-  <si>
-    <t>16:30-17:15</t>
-  </si>
-  <si>
-    <t>R 1</t>
-  </si>
-  <si>
-    <t>Large, Recorded</t>
-  </si>
-  <si>
-    <t>R 2</t>
-  </si>
-  <si>
-    <t>R 3</t>
-  </si>
-  <si>
-    <t>Recorded</t>
-  </si>
-  <si>
-    <t>R 4</t>
-  </si>
-  <si>
-    <t>R 5</t>
-  </si>
-  <si>
-    <t>Lab_room, Large, Recorded</t>
-  </si>
-  <si>
-    <t>Required timeslot tags</t>
-  </si>
-  <si>
-    <t>Preferred timeslot tags</t>
-  </si>
-  <si>
-    <t>Prohibited timeslot tags</t>
-  </si>
-  <si>
-    <t>Undesired timeslot tags</t>
-  </si>
-  <si>
-    <t>Required room tags</t>
-  </si>
-  <si>
-    <t>Preferred room tags</t>
-  </si>
-  <si>
-    <t>Prohibited room tags</t>
-  </si>
-  <si>
-    <t>Undesired room tags</t>
-  </si>
-  <si>
-    <t>Amy Cole</t>
-  </si>
-  <si>
-    <t>Beth Fox</t>
-  </si>
-  <si>
-    <t>Chad Green</t>
-  </si>
-  <si>
-    <t>Dan Jones</t>
-  </si>
-  <si>
-    <t>Elsa King</t>
-  </si>
-  <si>
-    <t>Flo Li</t>
-  </si>
-  <si>
-    <t>Gus Poe</t>
-  </si>
-  <si>
-    <t>Hugo Rye</t>
-  </si>
-  <si>
-    <t>Ivy Smith</t>
-  </si>
-  <si>
-    <t>Jay Watt</t>
-  </si>
-  <si>
-    <t>Amy Fox</t>
-  </si>
-  <si>
-    <t>Beth Green</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Title</t>
   </si>
   <si>
     <t>Speakers</t>
@@ -1302,7 +1305,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>76</v>
@@ -1325,13 +1328,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>65</v>
@@ -1404,7 +1407,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>76</v>
@@ -1427,13 +1430,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>65</v>
@@ -1506,7 +1509,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>76</v>
@@ -1529,13 +1532,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>65</v>
@@ -1574,7 +1577,7 @@
     <col min="1" max="1" width="15.99609375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="6.0859375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="6.0859375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="9.41796875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="10.29296875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="5.1484375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -2654,28 +2657,28 @@
         <v>111</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>112</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>90</v>
@@ -2702,10 +2705,10 @@
         <v>97</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>57</v>
@@ -2714,15 +2717,15 @@
         <v>58</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>64</v>
@@ -2731,22 +2734,22 @@
         <v>98</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>65</v>
@@ -2761,7 +2764,7 @@
         <v>65</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>65</v>
@@ -2790,10 +2793,10 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>64</v>
@@ -2802,22 +2805,22 @@
         <v>99</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>65</v>
@@ -2832,7 +2835,7 @@
         <v>65</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>65</v>
@@ -2861,10 +2864,10 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>67</v>
@@ -2873,22 +2876,22 @@
         <v>100</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>65</v>
@@ -2932,10 +2935,10 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>67</v>
@@ -2944,22 +2947,22 @@
         <v>101</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>65</v>
@@ -3003,34 +3006,34 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>65</v>
@@ -3074,34 +3077,34 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H7" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>65</v>
@@ -3145,10 +3148,10 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>67</v>
@@ -3157,22 +3160,22 @@
         <v>106</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H8" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>65</v>
@@ -3216,34 +3219,34 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H9" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>65</v>
@@ -3287,34 +3290,34 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H10" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>65</v>
@@ -3358,10 +3361,10 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>67</v>
@@ -3370,22 +3373,22 @@
         <v>102</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H11" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>65</v>
@@ -3429,10 +3432,10 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>67</v>
@@ -3441,22 +3444,22 @@
         <v>103</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H12" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>65</v>
@@ -3500,34 +3503,34 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H13" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>65</v>
@@ -3571,10 +3574,10 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>67</v>
@@ -3583,22 +3586,22 @@
         <v>106</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H14" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>65</v>
@@ -3642,34 +3645,34 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H15" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>65</v>
@@ -3713,34 +3716,34 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H16" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>65</v>
@@ -3784,34 +3787,34 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H17" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>65</v>
@@ -3855,10 +3858,10 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>67</v>
@@ -3867,22 +3870,22 @@
         <v>101</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H18" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>65</v>
@@ -3926,34 +3929,34 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H19" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>65</v>
@@ -4056,7 +4059,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>76</v>
@@ -4085,7 +4088,7 @@
         <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>65</v>
@@ -4250,7 +4253,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>76</v>
@@ -4348,7 +4351,7 @@
         <v>65</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>65</v>
@@ -4605,7 +4608,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>76</v>
@@ -4628,13 +4631,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>65</v>
@@ -4707,7 +4710,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
conf scheduling: talkTypeSet on timeslot and room
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
@@ -11,32 +11,16 @@
     <sheet name="Rooms" r:id="rId5" sheetId="3"/>
     <sheet name="Speakers" r:id="rId6" sheetId="4"/>
     <sheet name="Talks" r:id="rId7" sheetId="5"/>
-    <sheet name="Rooms view" r:id="rId8" sheetId="6"/>
-    <sheet name="Speakers view" r:id="rId9" sheetId="7"/>
-    <sheet name="Theme tracks view" r:id="rId10" sheetId="8"/>
-    <sheet name="Sectors view" r:id="rId11" sheetId="9"/>
-    <sheet name="Audience type view" r:id="rId12" sheetId="10"/>
-    <sheet name="Audience level view" r:id="rId13" sheetId="11"/>
-    <sheet name="Contents view" r:id="rId14" sheetId="12"/>
+    <sheet name="Score view" r:id="rId8" sheetId="6"/>
+    <sheet name="Rooms view" r:id="rId9" sheetId="7"/>
+    <sheet name="Speakers view" r:id="rId10" sheetId="8"/>
+    <sheet name="Theme tracks view" r:id="rId11" sheetId="9"/>
+    <sheet name="Sectors view" r:id="rId12" sheetId="10"/>
+    <sheet name="Audience type view" r:id="rId13" sheetId="11"/>
+    <sheet name="Audience level view" r:id="rId14" sheetId="12"/>
+    <sheet name="Contents view" r:id="rId15" sheetId="13"/>
   </sheets>
 </workbook>
-</file>
-
-<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="C3" authorId="0">
-      <text>
-        <t>S03: Intro to serverless Drools
-  Dan Jones
-  PINNED BY USER</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
@@ -73,7 +57,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -96,6 +80,23 @@
     <author/>
   </authors>
   <commentList>
+    <comment ref="C3" authorId="0">
+      <text>
+        <t>S03: Intro to serverless Drools
+  Dan Jones
+  PINNED BY USER</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
     <comment ref="C6" authorId="0">
       <text>
         <t>S03: Intro to serverless Drools
@@ -107,7 +108,7 @@
 </comments>
 </file>
 
-<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -125,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="214">
   <si>
     <t>Conference name</t>
   </si>
@@ -394,9 +395,6 @@
     <t>R 5</t>
   </si>
   <si>
-    <t>Lab_room, Large, Recorded</t>
-  </si>
-  <si>
     <t>Required timeslot tags</t>
   </si>
   <si>
@@ -517,9 +515,6 @@
     <t>en</t>
   </si>
   <si>
-    <t>Lab_room</t>
-  </si>
-  <si>
     <t>S01</t>
   </si>
   <si>
@@ -731,6 +726,24 @@
   </si>
   <si>
     <t>VertX</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>-34init</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Usable timeslots</t>
+  </si>
+  <si>
+    <t>Usable rooms</t>
+  </si>
+  <si>
+    <t>Usable sessions</t>
   </si>
   <si>
     <t>S03: Intro to serverless Drools
@@ -863,6 +876,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
 </file>
 
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
 </file>
@@ -1271,6 +1288,84 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
+    <col min="1" max="1" width="10.23828125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="11.86328125" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FCE94F"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
     <col min="1" max="1" width="14.1953125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.86328125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="11.86328125" customWidth="true" bestFit="true"/>
@@ -1305,7 +1400,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>76</v>
@@ -1328,13 +1423,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>65</v>
@@ -1359,7 +1454,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FCE94F"/>
@@ -1407,7 +1502,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>76</v>
@@ -1430,13 +1525,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>65</v>
@@ -1461,7 +1556,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FCE94F"/>
@@ -1509,7 +1604,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>76</v>
@@ -1532,13 +1627,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>65</v>
@@ -1718,13 +1813,14 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="6.48828125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="25.6328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="10.29296875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="15.51171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.86328125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="11.86328125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="11.86328125" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="11.86328125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.86328125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.86328125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1735,11 +1831,11 @@
         <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="E1" s="1" t="s">
         <v>65</v>
       </c>
@@ -1750,6 +1846,9 @@
         <v>65</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1758,24 +1857,27 @@
         <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1784,24 +1886,27 @@
         <v>82</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>65</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1810,24 +1915,27 @@
         <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>65</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1836,24 +1944,27 @@
         <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="F5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>65</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1862,24 +1973,27 @@
         <v>87</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="F6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>65</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1888,30 +2002,33 @@
         <v>88</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="F7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>65</v>
       </c>
       <c r="H7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="D1:I1"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>
@@ -1998,28 +2115,28 @@
         <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>76</v>
@@ -2042,7 +2159,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>65</v>
@@ -2089,7 +2206,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>65</v>
@@ -2136,7 +2253,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>65</v>
@@ -2183,7 +2300,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>65</v>
@@ -2230,7 +2347,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>65</v>
@@ -2277,7 +2394,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>65</v>
@@ -2324,7 +2441,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>65</v>
@@ -2371,7 +2488,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>65</v>
@@ -2418,7 +2535,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>65</v>
@@ -2465,7 +2582,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>65</v>
@@ -2512,7 +2629,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>65</v>
@@ -2559,7 +2676,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>65</v>
@@ -2651,64 +2768,64 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>57</v>
@@ -2717,40 +2834,40 @@
         <v>58</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="K2" s="2" t="s">
         <v>65</v>
       </c>
@@ -2764,7 +2881,7 @@
         <v>65</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>130</v>
+        <v>65</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>65</v>
@@ -2793,34 +2910,34 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>65</v>
@@ -2835,7 +2952,7 @@
         <v>65</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>130</v>
+        <v>65</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>65</v>
@@ -2864,34 +2981,34 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>65</v>
@@ -2935,34 +3052,34 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>65</v>
@@ -3006,34 +3123,34 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>65</v>
@@ -3077,34 +3194,34 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H7" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>65</v>
@@ -3148,34 +3265,34 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H8" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>65</v>
@@ -3219,34 +3336,34 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H9" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>65</v>
@@ -3290,34 +3407,34 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H10" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>65</v>
@@ -3361,34 +3478,34 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H11" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>65</v>
@@ -3432,34 +3549,34 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H12" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>65</v>
@@ -3503,34 +3620,34 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H13" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>65</v>
@@ -3574,34 +3691,34 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H14" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>65</v>
@@ -3645,34 +3762,34 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H15" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>65</v>
@@ -3716,34 +3833,34 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H16" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>65</v>
@@ -3787,34 +3904,34 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H17" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>65</v>
@@ -3858,34 +3975,34 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>65</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H18" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>65</v>
@@ -3929,34 +4046,34 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="G19" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H19" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>65</v>
@@ -4005,6 +4122,93 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FCE94F"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="9.4453125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="6.83984375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="16.22265625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="13.59375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="15.30078125" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FCE94F"/>
@@ -4059,7 +4263,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>76</v>
@@ -4088,7 +4292,7 @@
         <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>65</v>
@@ -4205,7 +4409,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FCE94F"/>
@@ -4253,7 +4457,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>76</v>
@@ -4276,7 +4480,7 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>65</v>
@@ -4299,7 +4503,7 @@
     </row>
     <row r="4" ht="15.0" customHeight="true">
       <c r="A4" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>65</v>
@@ -4322,7 +4526,7 @@
     </row>
     <row r="5" ht="15.0" customHeight="true">
       <c r="A5" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>65</v>
@@ -4345,13 +4549,13 @@
     </row>
     <row r="6" ht="15.0" customHeight="true">
       <c r="A6" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>65</v>
@@ -4368,7 +4572,7 @@
     </row>
     <row r="7" ht="15.0" customHeight="true">
       <c r="A7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>65</v>
@@ -4391,7 +4595,7 @@
     </row>
     <row r="8" ht="15.0" customHeight="true">
       <c r="A8" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>65</v>
@@ -4414,7 +4618,7 @@
     </row>
     <row r="9" ht="15.0" customHeight="true">
       <c r="A9" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>65</v>
@@ -4437,7 +4641,7 @@
     </row>
     <row r="10" ht="15.0" customHeight="true">
       <c r="A10" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>65</v>
@@ -4460,7 +4664,7 @@
     </row>
     <row r="11" ht="15.0" customHeight="true">
       <c r="A11" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>65</v>
@@ -4483,7 +4687,7 @@
     </row>
     <row r="12" ht="15.0" customHeight="true">
       <c r="A12" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>65</v>
@@ -4506,7 +4710,7 @@
     </row>
     <row r="13" ht="15.0" customHeight="true">
       <c r="A13" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>65</v>
@@ -4529,7 +4733,7 @@
     </row>
     <row r="14" ht="15.0" customHeight="true">
       <c r="A14" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>65</v>
@@ -4560,7 +4764,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FCE94F"/>
@@ -4608,7 +4812,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>76</v>
@@ -4631,13 +4835,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>65</v>
@@ -4660,82 +4864,4 @@
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <tabColor rgb="FCE94F"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="10.23828125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="11.86328125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="11.86328125" customWidth="true" bestFit="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells>
-    <mergeCell ref="B1:G1"/>
-  </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Parametrize hard constraints in ConferenceScheduling example
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="220">
   <si>
     <t>Conference name</t>
   </si>
@@ -256,10 +256,13 @@
     <t>Talk type of timeslot</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>Hard penalty per talk in a timeslot with an other talk type</t>
+    <t>Hard penalty per talk in a timeslot with another talk type</t>
+  </si>
+  <si>
+    <t>Talk type of room</t>
+  </si>
+  <si>
+    <t>Hard penalty per talk in a room with another talk type</t>
   </si>
   <si>
     <t>Room unavailable timeslot</t>
@@ -1186,143 +1189,154 @@
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="2" t="n">
+        <v>10000.0</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>10000.0</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>10000.0</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>34</v>
+      <c r="B29" s="2" t="n">
+        <v>1.0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>34</v>
+      <c r="B30" s="2" t="n">
+        <v>1.0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>34</v>
+      <c r="B33" s="2" t="n">
+        <v>1.0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1356,48 +1370,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1434,71 +1448,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1536,71 +1550,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1638,71 +1652,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1740,77 +1754,77 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -1845,13 +1859,13 @@
     <row r="1"/>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -1880,121 +1894,121 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2027,205 +2041,205 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2267,660 +2281,660 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2970,1351 +2984,1351 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S2" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S3" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S4" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S5" s="4" t="b">
         <v>1</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S6" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H7" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S7" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H8" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S8" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H9" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H10" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H11" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H12" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H13" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H14" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H15" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H16" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H17" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H18" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H19" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -4346,33 +4360,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2"/>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>2.0</v>
@@ -4389,7 +4403,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>16.0</v>
@@ -4407,7 +4421,7 @@
     <row r="6"/>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>18.0</v>
@@ -4460,163 +4474,163 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" ht="45.0" customHeight="true">
       <c r="A3" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" ht="45.0" customHeight="true">
       <c r="A4" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" ht="45.0" customHeight="true">
       <c r="A5" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" ht="45.0" customHeight="true">
       <c r="A6" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" ht="45.0" customHeight="true">
       <c r="A7" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -4661,324 +4675,324 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" ht="15.0" customHeight="true">
       <c r="A4" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" ht="15.0" customHeight="true">
       <c r="A5" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" ht="15.0" customHeight="true">
       <c r="A6" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="true">
       <c r="A7" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" ht="15.0" customHeight="true">
       <c r="A8" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" ht="15.0" customHeight="true">
       <c r="A9" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" ht="15.0" customHeight="true">
       <c r="A10" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" ht="15.0" customHeight="true">
       <c r="A11" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" ht="15.0" customHeight="true">
       <c r="A12" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" ht="15.0" customHeight="true">
       <c r="A13" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" ht="15.0" customHeight="true">
       <c r="A14" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -5016,71 +5030,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Genereate new examples data with the new constraints
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="228">
   <si>
     <t>Conference name</t>
   </si>
@@ -253,6 +253,12 @@
     <t>Talk undesired room tag</t>
   </si>
   <si>
+    <t>Same day talks</t>
+  </si>
+  <si>
+    <t>Soft penalty per common content/theme of 2 talks that are scheduled on different days</t>
+  </si>
+  <si>
     <t>Talk type of timeslot</t>
   </si>
   <si>
@@ -325,6 +331,18 @@
     <t>Talk prohibited room tag</t>
   </si>
   <si>
+    <t>Talk mutually-exclusive-talks tag</t>
+  </si>
+  <si>
+    <t>Hard penalty per two talks that share the same Mutually exclusive talks tag that are scheduled in overlapping timeslots</t>
+  </si>
+  <si>
+    <t>Talk prerequisite talks</t>
+  </si>
+  <si>
+    <t>Hard penalty per talk that is scheduled before any of its prerequisite talks</t>
+  </si>
+  <si>
     <t>Day</t>
   </si>
   <si>
@@ -512,6 +530,12 @@
   </si>
   <si>
     <t>Language</t>
+  </si>
+  <si>
+    <t>Mutually exclusive talks tags</t>
+  </si>
+  <si>
+    <t>Prerequisite talks codes</t>
   </si>
   <si>
     <t>Pinned by user</t>
@@ -1184,18 +1208,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20"/>
-    <row r="21">
-      <c r="A21" s="1" t="s">
+    <row r="20">
+      <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="2" t="n">
-        <v>10000.0</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="B20" s="2" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>34</v>
       </c>
     </row>
+    <row r="21"/>
     <row r="22">
       <c r="A22" s="1" t="s">
         <v>35</v>
@@ -1223,7 +1247,7 @@
         <v>39</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>10.0</v>
+        <v>10000.0</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>40</v>
@@ -1234,7 +1258,7 @@
         <v>41</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>42</v>
@@ -1281,12 +1305,12 @@
         <v>1.0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B30" s="2" t="n">
         <v>1.0</v>
@@ -1297,13 +1321,13 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B31" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32">
@@ -1325,18 +1349,51 @@
         <v>1.0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B34" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1370,48 +1427,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1448,71 +1505,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1550,71 +1607,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1652,71 +1709,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1754,77 +1811,77 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -1859,13 +1916,13 @@
     <row r="1"/>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -1894,121 +1951,121 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2041,205 +2098,205 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2281,660 +2338,660 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2975,1360 +3032,1476 @@
     <col min="16" max="16" width="22.20703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="23.125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="22.84375" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" width="16.65234375" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="16.14453125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="6.3984375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="6.32421875" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="7.02734375" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" width="31.2734375" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="26.23046875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="16.65234375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="16.14453125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="6.3984375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="6.32421875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="7.02734375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>58</v>
+        <v>128</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>59</v>
+        <v>129</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>122</v>
+        <v>64</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S2" s="2" t="b">
+        <v>72</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="T2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="V2" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S3" s="2" t="b">
+        <v>72</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="T3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="V3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S4" s="2" t="b">
+        <v>72</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="T4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="V4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S5" s="4" t="b">
+        <v>72</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U5" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="T5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="V5" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>83</v>
+        <v>69</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S6" s="2" t="b">
+        <v>72</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="T6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="V6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="H7" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S7" s="2" t="b">
+        <v>72</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U7" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="T7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="V7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="H8" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S8" s="2" t="b">
+        <v>72</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U8" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="T8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="V8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="H9" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S9" s="2" t="b">
+        <v>72</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U9" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="T9" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="V9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="H10" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S10" s="2" t="b">
+        <v>72</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U10" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="T10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U10" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="V10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="H11" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S11" s="2" t="b">
+        <v>72</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U11" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="T11" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U11" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="V11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y11" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="H12" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S12" s="2" t="b">
+        <v>72</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U12" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="T12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="V12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="H13" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S13" s="2" t="b">
+        <v>72</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U13" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="T13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="V13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y13" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="H14" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S14" s="2" t="b">
+        <v>72</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U14" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="T14" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="V14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="H15" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S15" s="2" t="b">
+        <v>72</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U15" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="T15" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U15" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="V15" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="X15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y15" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="H16" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S16" s="2" t="b">
+        <v>72</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U16" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="T16" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U16" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="V16" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="X16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y16" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="H17" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S17" s="2" t="b">
+        <v>72</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U17" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="T17" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U17" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="V17" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="X17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="H18" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S18" s="2" t="b">
+        <v>72</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U18" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="T18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U18" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="V18" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="X18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y18" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="H19" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S19" s="2" t="b">
+        <v>72</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U19" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="T19" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U19" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="V19" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="X19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y19" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -4360,33 +4533,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2"/>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>2.0</v>
@@ -4403,7 +4576,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>16.0</v>
@@ -4421,7 +4594,7 @@
     <row r="6"/>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>18.0</v>
@@ -4474,163 +4647,163 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" ht="45.0" customHeight="true">
       <c r="A3" s="2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" ht="45.0" customHeight="true">
       <c r="A4" s="2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" ht="45.0" customHeight="true">
       <c r="A5" s="2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" ht="45.0" customHeight="true">
       <c r="A6" s="2" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" ht="45.0" customHeight="true">
       <c r="A7" s="2" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -4675,324 +4848,324 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" ht="15.0" customHeight="true">
       <c r="A4" s="2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" ht="15.0" customHeight="true">
       <c r="A5" s="2" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" ht="15.0" customHeight="true">
       <c r="A6" s="2" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="true">
       <c r="A7" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" ht="15.0" customHeight="true">
       <c r="A8" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" ht="15.0" customHeight="true">
       <c r="A9" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" ht="15.0" customHeight="true">
       <c r="A10" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" ht="15.0" customHeight="true">
       <c r="A11" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" ht="15.0" customHeight="true">
       <c r="A12" s="2" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" ht="15.0" customHeight="true">
       <c r="A13" s="2" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" ht="15.0" customHeight="true">
       <c r="A14" s="2" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -5030,71 +5203,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add capacity field to class Room
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="1" state="visible" r:id="rId2"/>
@@ -47,7 +47,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">S11: Understand mobile Errai
+          <t xml:space="preserve">S10: Prepare for streaming GWT
     Dan Jones
 PINNED BY USER
 </t>
@@ -72,7 +72,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">S11: Understand mobile Errai
+          <t xml:space="preserve">S10: Prepare for streaming GWT
     Dan Jones
 PINNED BY USER
 </t>
@@ -97,7 +97,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">S11: Understand mobile Errai
+          <t xml:space="preserve">S10: Prepare for streaming GWT
     Dan Jones
 PINNED BY USER
 </t>
@@ -122,7 +122,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">S11: Understand mobile Errai
+          <t xml:space="preserve">S10: Prepare for streaming GWT
     Dan Jones
 PINNED BY USER
 </t>
@@ -147,7 +147,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">S11: Understand mobile Errai
+          <t xml:space="preserve">S10: Prepare for streaming GWT
     Dan Jones
 PINNED BY USER
 </t>
@@ -172,7 +172,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">S11: Understand mobile Errai
+          <t xml:space="preserve">S10: Prepare for streaming GWT
     Dan Jones
 PINNED BY USER
 </t>
@@ -197,7 +197,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">S11: Understand mobile Errai
+          <t xml:space="preserve">S10: Prepare for streaming GWT
     Dan Jones
 PINNED BY USER
 </t>
@@ -209,7 +209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="231">
   <si>
     <t xml:space="preserve">Conference name</t>
   </si>
@@ -457,6 +457,9 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Capacity</t>
+  </si>
+  <si>
     <t xml:space="preserve">10:15-12:15</t>
   </si>
   <si>
@@ -487,12 +490,12 @@
     <t xml:space="preserve">R 3</t>
   </si>
   <si>
+    <t xml:space="preserve">R 4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Recorded</t>
   </si>
   <si>
-    <t xml:space="preserve">R 4</t>
-  </si>
-  <si>
     <t xml:space="preserve">R 5</t>
   </si>
   <si>
@@ -613,231 +616,234 @@
     <t xml:space="preserve">Hands on real-time OpenShift</t>
   </si>
   <si>
+    <t xml:space="preserve">Amy Cole, Beth Fox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Big Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business analysts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenShift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advanced containerized WildFly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chad Green, Dan Jones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Managers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WildFly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learn virtualized Spring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IoT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programmers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intro to serverless Drools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Big Data, Culture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discover AI-driven OptaPlanner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gus Poe, Hugo Rye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OptaPlanner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mastering machine learning jBPM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middleware, Modern Web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Financial services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jBPM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuning IOT-driven Camel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Government</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Building deep learning XStream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amy Fox, Beth Green, Amy Cole</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cloud</t>
   </si>
   <si>
-    <t xml:space="preserve">Government</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Business analysts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OpenShift</t>
-  </si>
-  <si>
-    <t xml:space="preserve">en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Advanced containerized WildFly</t>
+    <t xml:space="preserve">XStream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Securing scalable Docker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Security, Culture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Docker, Kubernetes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug enterprise Hibernate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Culture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telecommunications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hibernate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prepare for streaming GWT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GWT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understand mobile Errai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elsa King, Flo Li</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artificial Intelligence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Errai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Applying modern Angular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grok distributed Weld</t>
   </si>
   <si>
     <t xml:space="preserve">Middleware, Security</t>
   </si>
   <si>
-    <t xml:space="preserve">Managers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WildFly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Learn virtualized Spring</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chad Green, Dan Jones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Big Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spring</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intro to serverless Drools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Discover AI-driven OptaPlanner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Artificial Intelligence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OptaPlanner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mastering machine learning jBPM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IoT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Healthcare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jBPM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tuning IOT-driven Camel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Programmers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Building deep learning XStream</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Artificial Intelligence, Security</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Financial services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XStream</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Securing scalable Docker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jay Watt, Amy Fox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Culture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Docker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Debug enterprise Hibernate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beth Green, Amy Cole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hibernate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prepare for streaming GWT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beth Fox, Chad Green</t>
+    <t xml:space="preserve">Weld</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Troubleshooting reliable RestEasy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile, Culture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RestEasy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using secure Android</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deliver stable Tensorflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud, Culture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tensorflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement platform-independent VertX</t>
   </si>
   <si>
     <t xml:space="preserve">Middleware</t>
   </si>
   <si>
-    <t xml:space="preserve">GWT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Understand mobile Errai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Errai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Applying modern Angular</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud, Middleware</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Angular</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grok distributed Weld</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flo Li, Gus Poe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weld</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Troubleshooting reliable RestEasy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Security</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RestEasy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Using secure Android</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ivy Smith, Jay Watt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deliver stable Tensorflow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tensorflow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implement platform-independent VertX</t>
-  </si>
-  <si>
     <t xml:space="preserve">VertX</t>
   </si>
   <si>
@@ -862,14 +868,14 @@
     <t xml:space="preserve">Total</t>
   </si>
   <si>
-    <t xml:space="preserve">S11: Understand mobile Errai
+    <t xml:space="preserve">S10: Prepare for streaming GWT
   Dan Jones</t>
   </si>
   <si>
     <t xml:space="preserve">Speaker</t>
   </si>
   <si>
-    <t xml:space="preserve">S11 @ R 1</t>
+    <t xml:space="preserve">S10 @ R 1</t>
   </si>
   <si>
     <t xml:space="preserve">Theme track tag</t>
@@ -887,7 +893,7 @@
     <t xml:space="preserve">Content tag</t>
   </si>
   <si>
-    <t xml:space="preserve">S11 (level 1)</t>
+    <t xml:space="preserve">S10 (level 1)</t>
   </si>
   <si>
     <t xml:space="preserve">Constraint match</t>
@@ -1098,7 +1104,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="V6:V12 A1"/>
+      <selection pane="bottomRight" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1515,7 +1521,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="V6:V12 A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1538,25 +1544,25 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1586,12 +1592,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="V6:V12 A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="13.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.67"/>
   </cols>
@@ -1609,34 +1615,34 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="5" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1671,7 +1677,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="V6:V12 A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1694,34 +1700,34 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="5" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1756,7 +1762,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="V6:V12 A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1779,34 +1785,34 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="5" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1841,7 +1847,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="V6:V12 A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1864,44 +1870,44 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="5" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -1932,7 +1938,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="V6:V12 A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1945,13 +1951,13 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -1977,7 +1983,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="V6:V12 A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2113,23 +2119,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="V6:V12 A1"/>
+      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="4" style="0" width="13.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="5" style="0" width="13.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2150,13 +2157,13 @@
         <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>83</v>
@@ -2173,89 +2180,107 @@
       <c r="I2" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J2" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>240</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>630</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>490</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2283,7 +2308,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="V6:V12 A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2325,51 +2350,51 @@
         <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2388,7 +2413,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2407,16 +2432,14 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
-        <v>92</v>
-      </c>
+      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -2428,7 +2451,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2447,7 +2470,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2466,7 +2489,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2476,25 +2499,23 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
-        <v>92</v>
-      </c>
+      <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -2506,7 +2527,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2525,7 +2546,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2535,25 +2556,23 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2" t="s">
-        <v>92</v>
-      </c>
+      <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -2565,7 +2584,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2584,7 +2603,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2622,12 +2641,12 @@
   </sheetPr>
   <dimension ref="A1:AA19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U8" activeCellId="1" sqref="V6:V12 U8"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2635,12 +2654,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="25.4"/>
@@ -2664,76 +2683,76 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>64</v>
@@ -2742,39 +2761,37 @@
         <v>65</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>135</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -2787,10 +2804,10 @@
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2" t="n">
-        <v>663</v>
+        <v>623</v>
       </c>
       <c r="V2" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W2" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -2803,32 +2820,34 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F3" s="2"/>
+        <v>136</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="G3" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -2841,10 +2860,10 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2" t="n">
-        <v>474</v>
+        <v>291</v>
       </c>
       <c r="V3" s="2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W3" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -2857,32 +2876,32 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>146</v>
+        <v>108</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -2895,10 +2914,10 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2" t="n">
-        <v>362</v>
+        <v>214</v>
       </c>
       <c r="V4" s="2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W4" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -2911,32 +2930,32 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -2949,10 +2968,10 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
       <c r="U5" s="2" t="n">
-        <v>82</v>
+        <v>761</v>
       </c>
       <c r="V5" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W5" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -2963,36 +2982,34 @@
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>135</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -3005,7 +3022,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2" t="n">
-        <v>841</v>
+        <v>388</v>
       </c>
       <c r="V6" s="2" t="n">
         <v>2</v>
@@ -3019,36 +3036,36 @@
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -3061,10 +3078,10 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2" t="n">
-        <v>957</v>
+        <v>798</v>
       </c>
       <c r="V7" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -3075,34 +3092,36 @@
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F8" s="2"/>
+        <v>148</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>166</v>
+      </c>
       <c r="G8" s="2" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -3115,10 +3134,10 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2" t="n">
-        <v>628</v>
+        <v>401</v>
       </c>
       <c r="V8" s="2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W8" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -3129,36 +3148,34 @@
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>111</v>
+        <v>170</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>168</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="H9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -3171,10 +3188,10 @@
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2" t="n">
-        <v>509</v>
+        <v>720</v>
       </c>
       <c r="V9" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W9" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -3185,34 +3202,34 @@
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>172</v>
+        <v>105</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -3225,10 +3242,10 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2" t="n">
-        <v>349</v>
+        <v>55</v>
       </c>
       <c r="V10" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W10" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -3239,34 +3256,36 @@
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>177</v>
+        <v>106</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F11" s="2"/>
+        <v>179</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>180</v>
+      </c>
       <c r="G11" s="2" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -3279,10 +3298,10 @@
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2" t="n">
-        <v>166</v>
+        <v>333</v>
       </c>
       <c r="V11" s="2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W11" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -3293,34 +3312,34 @@
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>181</v>
+        <v>107</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -3333,48 +3352,58 @@
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2" t="n">
-        <v>435</v>
+        <v>546</v>
       </c>
       <c r="V12" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="W12" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="X12" s="2"/>
-      <c r="Y12" s="2"/>
-      <c r="Z12" s="2"/>
-      <c r="AA12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2</v>
+      </c>
+      <c r="W12" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>106</v>
+        <v>187</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F13" s="2"/>
+        <v>188</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="G13" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -3387,58 +3416,48 @@
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2" t="n">
-        <v>429</v>
+        <v>785</v>
       </c>
       <c r="V13" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="W13" s="2" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="W13" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="X13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y13" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA13" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>168</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="F14" s="2"/>
       <c r="G14" s="2" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="H14" s="2" t="n">
         <v>1</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -3451,7 +3470,7 @@
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2" t="n">
-        <v>340</v>
+        <v>245</v>
       </c>
       <c r="V14" s="2" t="n">
         <v>1</v>
@@ -3467,32 +3486,34 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>193</v>
+        <v>111</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="F15" s="2"/>
+        <v>195</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="G15" s="2" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -3505,10 +3526,10 @@
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2" t="n">
+        <v>156</v>
+      </c>
+      <c r="V15" s="2" t="n">
         <v>1</v>
-      </c>
-      <c r="V15" s="2" t="n">
-        <v>2</v>
       </c>
       <c r="W15" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -3521,32 +3542,32 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="H16" s="2" t="n">
         <v>3</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -3559,10 +3580,10 @@
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
       <c r="U16" s="2" t="n">
-        <v>957</v>
+        <v>318</v>
       </c>
       <c r="V16" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W16" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -3575,32 +3596,32 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>202</v>
+        <v>113</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>203</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -3613,10 +3634,10 @@
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2" t="n">
-        <v>288</v>
+        <v>56</v>
       </c>
       <c r="V17" s="2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W17" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -3638,23 +3659,23 @@
         <v>73</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -3667,7 +3688,7 @@
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2" t="n">
-        <v>39</v>
+        <v>596</v>
       </c>
       <c r="V18" s="2" t="n">
         <v>3</v>
@@ -3683,32 +3704,32 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>177</v>
+        <v>115</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>173</v>
+        <v>210</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -3721,10 +3742,10 @@
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2" t="n">
-        <v>458</v>
+        <v>701</v>
       </c>
       <c r="V19" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W19" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -3759,7 +3780,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="V6:V12 A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3774,27 +3795,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3833,7 +3854,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>18</v>
@@ -3872,7 +3893,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="V6:V12 A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3895,34 +3916,34 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="4"/>
@@ -3931,7 +3952,7 @@
     </row>
     <row r="4" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="2"/>
@@ -3942,7 +3963,7 @@
     </row>
     <row r="5" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="2"/>
@@ -3964,7 +3985,7 @@
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="4"/>
@@ -4001,7 +4022,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="V6:V12 A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4024,30 +4045,30 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -4058,7 +4079,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -4069,7 +4090,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -4080,11 +4101,11 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="5" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -4093,7 +4114,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -4104,18 +4125,18 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+        <v>109</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -4126,7 +4147,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4137,18 +4158,18 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+        <v>112</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -4159,7 +4180,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -4170,7 +4191,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -4207,12 +4228,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="V6:V12 A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="13.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.67"/>
   </cols>
@@ -4230,34 +4251,34 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="5" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>

</xml_diff>

<commit_message>
Change tag to tags in rules and genereate new example xlsx files
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
@@ -36,6 +36,8 @@
         <t xml:space="preserve">S10: Prepare for streaming GWT
     Dan Jones
 PINNED BY USER
+-10soft total
+    -10soft for 1 Crowd controls
 </t>
       </text>
     </comment>
@@ -54,6 +56,8 @@
         <t xml:space="preserve">S10: Prepare for streaming GWT
     Dan Jones
 PINNED BY USER
+-10soft total
+    -10soft for 1 Crowd controls
 </t>
       </text>
     </comment>
@@ -72,6 +76,8 @@
         <t xml:space="preserve">S10: Prepare for streaming GWT
     Dan Jones
 PINNED BY USER
+-10soft total
+    -10soft for 1 Crowd controls
 </t>
       </text>
     </comment>
@@ -90,6 +96,8 @@
         <t xml:space="preserve">S10: Prepare for streaming GWT
     Dan Jones
 PINNED BY USER
+-10soft total
+    -10soft for 1 Crowd controls
 </t>
       </text>
     </comment>
@@ -108,6 +116,8 @@
         <t xml:space="preserve">S10: Prepare for streaming GWT
     Dan Jones
 PINNED BY USER
+-10soft total
+    -10soft for 1 Crowd controls
 </t>
       </text>
     </comment>
@@ -126,6 +136,8 @@
         <t xml:space="preserve">S10: Prepare for streaming GWT
     Dan Jones
 PINNED BY USER
+-10soft total
+    -10soft for 1 Crowd controls
 </t>
       </text>
     </comment>
@@ -144,6 +156,8 @@
         <t xml:space="preserve">S10: Prepare for streaming GWT
     Dan Jones
 PINNED BY USER
+-10soft total
+    -10soft for 1 Crowd controls
 </t>
       </text>
     </comment>
@@ -152,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="238">
   <si>
     <t>Conference name</t>
   </si>
@@ -265,6 +279,12 @@
     <t>Soft penalty per 2 talks where the less popular one (has lower number of likes) is assigned a larger room than the more popular talk</t>
   </si>
   <si>
+    <t>Crowd control</t>
+  </si>
+  <si>
+    <t>Soft penalty per talks with crowd control risk greater than zero that are not in pairs</t>
+  </si>
+  <si>
     <t>Talk type of timeslot</t>
   </si>
   <si>
@@ -802,7 +822,7 @@
     <t>Score</t>
   </si>
   <si>
-    <t>-34init</t>
+    <t>-34init/-10soft</t>
   </si>
   <si>
     <t>Count</t>
@@ -855,6 +875,12 @@
   </si>
   <si>
     <t>Total score</t>
+  </si>
+  <si>
+    <t>-10soft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    S10</t>
   </si>
 </sst>
 </file>
@@ -1248,18 +1274,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22"/>
-    <row r="23">
-      <c r="A23" s="1" t="s">
+    <row r="22">
+      <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="2" t="n">
-        <v>10000.0</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="B22" s="2" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>38</v>
       </c>
     </row>
+    <row r="23"/>
     <row r="24">
       <c r="A24" s="1" t="s">
         <v>39</v>
@@ -1287,7 +1313,7 @@
         <v>43</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>10.0</v>
+        <v>10000.0</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>44</v>
@@ -1298,7 +1324,7 @@
         <v>45</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>46</v>
@@ -1345,12 +1371,12 @@
         <v>1.0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B32" s="2" t="n">
         <v>1.0</v>
@@ -1361,13 +1387,13 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B33" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34">
@@ -1389,12 +1415,12 @@
         <v>1.0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B36" s="2" t="n">
         <v>1.0</v>
@@ -1405,13 +1431,13 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B37" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38">
@@ -1423,6 +1449,17 @@
       </c>
       <c r="C38" s="1" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1456,48 +1493,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1534,71 +1571,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1636,71 +1673,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1738,71 +1775,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1840,77 +1877,77 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -1945,14 +1982,33 @@
     <row r="1"/>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>233</v>
-      </c>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1980,121 +2036,121 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2128,226 +2184,226 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>60.0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>240.0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>630.0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>70.0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>490.0</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2389,660 +2445,660 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -3096,147 +3152,147 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U2" s="2" t="n">
         <v>623.0</v>
@@ -3248,78 +3304,78 @@
         <v>0</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U3" s="2" t="n">
         <v>291.0</v>
@@ -3331,78 +3387,78 @@
         <v>0</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U4" s="2" t="n">
         <v>214.0</v>
@@ -3414,78 +3470,78 @@
         <v>0</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U5" s="2" t="n">
         <v>761.0</v>
@@ -3497,78 +3553,78 @@
         <v>0</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U6" s="2" t="n">
         <v>388.0</v>
@@ -3580,78 +3636,78 @@
         <v>0</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H7" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U7" s="2" t="n">
         <v>798.0</v>
@@ -3663,78 +3719,78 @@
         <v>0</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA7" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H8" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U8" s="2" t="n">
         <v>401.0</v>
@@ -3746,78 +3802,78 @@
         <v>0</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H9" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U9" s="2" t="n">
         <v>720.0</v>
@@ -3829,78 +3885,78 @@
         <v>0</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Y9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA9" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H10" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U10" s="2" t="n">
         <v>55.0</v>
@@ -3912,78 +3968,78 @@
         <v>0</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Y10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H11" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U11" s="2" t="n">
         <v>333.0</v>
@@ -3995,78 +4051,78 @@
         <v>0</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H12" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U12" s="2" t="n">
         <v>546.0</v>
@@ -4078,78 +4134,78 @@
         <v>1</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AA12" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H13" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U13" s="2" t="n">
         <v>785.0</v>
@@ -4161,78 +4217,78 @@
         <v>0</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Y13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>191</v>
-      </c>
       <c r="F14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H14" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U14" s="2" t="n">
         <v>245.0</v>
@@ -4244,78 +4300,78 @@
         <v>0</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Y14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA14" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H15" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U15" s="2" t="n">
         <v>156.0</v>
@@ -4327,78 +4383,78 @@
         <v>0</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Y15" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z15" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA15" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H16" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U16" s="2" t="n">
         <v>318.0</v>
@@ -4410,78 +4466,78 @@
         <v>0</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Y16" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z16" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA16" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H17" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U17" s="2" t="n">
         <v>56.0</v>
@@ -4493,78 +4549,78 @@
         <v>0</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H18" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U18" s="2" t="n">
         <v>596.0</v>
@@ -4576,78 +4632,78 @@
         <v>0</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Y18" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z18" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA18" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H19" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U19" s="2" t="n">
         <v>701.0</v>
@@ -4659,16 +4715,16 @@
         <v>0</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Y19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -4692,7 +4748,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="10.78515625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="7.27734375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="13.98828125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="18.4296875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="15.25" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="17.625" customWidth="true" bestFit="true"/>
@@ -4700,33 +4756,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2"/>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>2.0</v>
@@ -4743,7 +4799,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>16.0</v>
@@ -4761,7 +4817,7 @@
     <row r="6"/>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>18.0</v>
@@ -4814,163 +4870,163 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" ht="45.0" customHeight="true">
       <c r="A3" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" ht="45.0" customHeight="true">
       <c r="A4" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" ht="45.0" customHeight="true">
       <c r="A5" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" ht="45.0" customHeight="true">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" ht="45.0" customHeight="true">
       <c r="A7" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -5015,324 +5071,324 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" ht="15.0" customHeight="true">
       <c r="A4" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" ht="15.0" customHeight="true">
       <c r="A5" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" ht="15.0" customHeight="true">
       <c r="A6" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="true">
       <c r="A7" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" ht="15.0" customHeight="true">
       <c r="A8" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" ht="15.0" customHeight="true">
       <c r="A9" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" ht="15.0" customHeight="true">
       <c r="A10" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" ht="15.0" customHeight="true">
       <c r="A11" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" ht="15.0" customHeight="true">
       <c r="A12" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" ht="15.0" customHeight="true">
       <c r="A13" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" ht="15.0" customHeight="true">
       <c r="A14" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -5370,71 +5426,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add publishedTimeslot and publishedRoom fields to class Talk
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="242">
   <si>
     <t>Conference name</t>
   </si>
@@ -580,6 +580,18 @@
   </si>
   <si>
     <t>Room</t>
+  </si>
+  <si>
+    <t>Published Timeslot</t>
+  </si>
+  <si>
+    <t>Published Start</t>
+  </si>
+  <si>
+    <t>Published End</t>
+  </si>
+  <si>
+    <t>Published Room</t>
   </si>
   <si>
     <t>S00</t>
@@ -1042,7 +1054,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="1.0" ySplit="3.0" state="frozen" topLeftCell="B4" activePane="bottomRight"/>
@@ -1473,7 +1485,7 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -1516,7 +1528,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>88</v>
@@ -1551,7 +1563,7 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -1594,7 +1606,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>88</v>
@@ -1617,13 +1629,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>76</v>
@@ -1653,7 +1665,7 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -1719,13 +1731,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>230</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>226</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>76</v>
@@ -1755,7 +1767,7 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -1798,7 +1810,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>88</v>
@@ -1821,13 +1833,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>76</v>
@@ -1857,7 +1869,7 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -1923,13 +1935,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>76</v>
@@ -1942,12 +1954,6 @@
       </c>
       <c r="G3" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -1965,50 +1971,58 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <pane xSplit="1.0" ySplit="3.0" state="frozen" topLeftCell="B4" activePane="bottomRight"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="19.0703125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="13.73828125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="13.98828125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.66015625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1"/>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -2018,7 +2032,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3.0" ySplit="1.0" state="frozen" topLeftCell="D2" activePane="bottomRight"/>
@@ -2161,7 +2175,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -2417,7 +2431,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -3112,7 +3126,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AF19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -3148,6 +3162,10 @@
     <col min="25" max="25" width="6.3984375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="6.32421875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="7.02734375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="20.8828125" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.20703125" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="15.86328125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="17.8359375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3232,37 +3250,49 @@
       <c r="AA1" s="1" t="s">
         <v>137</v>
       </c>
+      <c r="AB1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>75</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>76</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>76</v>
@@ -3315,37 +3345,49 @@
       <c r="AA2" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="AB2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>75</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>76</v>
@@ -3398,13 +3440,25 @@
       <c r="AA3" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="AB3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>78</v>
@@ -3413,22 +3467,22 @@
         <v>113</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>76</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>76</v>
@@ -3481,13 +3535,25 @@
       <c r="AA4" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="AB4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>78</v>
@@ -3496,22 +3562,22 @@
         <v>114</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>76</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>76</v>
@@ -3564,37 +3630,49 @@
       <c r="AA5" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="AB5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>78</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>76</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>76</v>
@@ -3647,13 +3725,25 @@
       <c r="AA6" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="AB6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>78</v>
@@ -3662,22 +3752,22 @@
         <v>117</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H7" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>76</v>
@@ -3730,13 +3820,25 @@
       <c r="AA7" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="AB7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>78</v>
@@ -3745,22 +3847,22 @@
         <v>118</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H8" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>76</v>
@@ -3813,37 +3915,49 @@
       <c r="AA8" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="AB8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>78</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>76</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="H9" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>76</v>
@@ -3896,13 +4010,25 @@
       <c r="AA9" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="AB9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE9" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>78</v>
@@ -3911,22 +4037,22 @@
         <v>110</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>76</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H10" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>76</v>
@@ -3979,13 +4105,25 @@
       <c r="AA10" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="AB10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE10" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>78</v>
@@ -3994,22 +4132,22 @@
         <v>111</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="H11" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>76</v>
@@ -4062,13 +4200,25 @@
       <c r="AA11" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="AB11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE11" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>78</v>
@@ -4077,22 +4227,22 @@
         <v>112</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>76</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H12" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>76</v>
@@ -4145,37 +4295,49 @@
       <c r="AA12" s="2" t="s">
         <v>94</v>
       </c>
+      <c r="AB12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE12" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>78</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="H13" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>76</v>
@@ -4228,13 +4390,25 @@
       <c r="AA13" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="AB13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE13" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>78</v>
@@ -4243,22 +4417,22 @@
         <v>115</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>76</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="H14" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>76</v>
@@ -4311,13 +4485,25 @@
       <c r="AA14" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="AB14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE14" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>78</v>
@@ -4326,22 +4512,22 @@
         <v>116</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="H15" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>76</v>
@@ -4394,13 +4580,25 @@
       <c r="AA15" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="AB15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE15" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>78</v>
@@ -4409,22 +4607,22 @@
         <v>117</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>76</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H16" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>76</v>
@@ -4477,13 +4675,25 @@
       <c r="AA16" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="AB16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE16" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>78</v>
@@ -4492,22 +4702,22 @@
         <v>118</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>76</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="H17" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>76</v>
@@ -4560,13 +4770,25 @@
       <c r="AA17" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="AB17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE17" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>78</v>
@@ -4575,22 +4797,22 @@
         <v>119</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>76</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="H18" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>76</v>
@@ -4643,13 +4865,25 @@
       <c r="AA18" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="AB18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE18" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>78</v>
@@ -4658,22 +4892,22 @@
         <v>120</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>76</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H19" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>76</v>
@@ -4724,6 +4958,18 @@
         <v>76</v>
       </c>
       <c r="AA19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE19" s="2" t="s">
         <v>76</v>
       </c>
     </row>
@@ -4738,7 +4984,7 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
@@ -4756,10 +5002,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2"/>
@@ -4768,16 +5014,16 @@
         <v>123</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4">
@@ -4817,7 +5063,7 @@
     <row r="6"/>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>18.0</v>
@@ -4843,7 +5089,7 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -4922,7 +5168,7 @@
         <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>76</v>
@@ -5044,7 +5290,7 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -5094,7 +5340,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>88</v>
@@ -5192,7 +5438,7 @@
         <v>76</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>76</v>
@@ -5406,7 +5652,7 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -5449,7 +5695,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>88</v>
@@ -5472,13 +5718,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
Generate new files with new constraint
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="251">
   <si>
     <t>Conference name</t>
   </si>
@@ -400,6 +400,12 @@
   </si>
   <si>
     <t>Hard penalty per talk that is scheduled before any of its prerequisite talks</t>
+  </si>
+  <si>
+    <t>Consecutive talks pause</t>
+  </si>
+  <si>
+    <t>Hard penalty per two consecutive talks for the same speaker with a pause less than minimum pause</t>
   </si>
   <si>
     <t>Day</t>
@@ -1162,7 +1168,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="1.0" ySplit="3.0" state="frozen" topLeftCell="B4" activePane="bottomRight"/>
@@ -1614,6 +1620,17 @@
       </c>
       <c r="C43" s="1" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1647,48 +1664,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1725,71 +1742,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1827,71 +1844,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1929,71 +1946,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2031,71 +2048,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2129,22 +2146,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2"/>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4">
@@ -2153,15 +2170,15 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -2192,58 +2209,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" ht="45.0" customHeight="true">
       <c r="A2" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" ht="45.0" customHeight="true">
       <c r="A3" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" ht="45.0" customHeight="true">
       <c r="A4" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" ht="45.0" customHeight="true">
       <c r="A5" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" ht="45.0" customHeight="true">
       <c r="A6" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" ht="45.0" customHeight="true">
       <c r="A7" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2273,121 +2290,121 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2421,226 +2438,226 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>60.0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>240.0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>630.0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>70.0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>490.0</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2682,660 +2699,660 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -3393,159 +3410,159 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U2" s="2" t="n">
         <v>623.0</v>
@@ -3557,90 +3574,90 @@
         <v>0</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U3" s="2" t="n">
         <v>291.0</v>
@@ -3652,90 +3669,90 @@
         <v>0</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U4" s="2" t="n">
         <v>214.0</v>
@@ -3747,90 +3764,90 @@
         <v>0</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U5" s="2" t="n">
         <v>761.0</v>
@@ -3842,90 +3859,90 @@
         <v>0</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U6" s="2" t="n">
         <v>388.0</v>
@@ -3937,90 +3954,90 @@
         <v>0</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H7" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U7" s="2" t="n">
         <v>798.0</v>
@@ -4032,90 +4049,90 @@
         <v>0</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AA7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AB7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AC7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AE7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H8" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U8" s="2" t="n">
         <v>401.0</v>
@@ -4127,90 +4144,90 @@
         <v>0</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AA8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AB8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AC8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AE8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H9" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U9" s="2" t="n">
         <v>720.0</v>
@@ -4222,90 +4239,90 @@
         <v>0</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AA9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AC9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AE9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H10" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U10" s="2" t="n">
         <v>55.0</v>
@@ -4317,90 +4334,90 @@
         <v>0</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AA10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AE10" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H11" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U11" s="2" t="n">
         <v>333.0</v>
@@ -4412,90 +4429,90 @@
         <v>0</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Z11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AB11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AC11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AE11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H12" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U12" s="2" t="n">
         <v>546.0</v>
@@ -4507,90 +4524,90 @@
         <v>1</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="AA12" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AB12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AC12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AE12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H13" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U13" s="2" t="n">
         <v>785.0</v>
@@ -4602,90 +4619,90 @@
         <v>0</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Z13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AA13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AB13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AC13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AE13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>203</v>
-      </c>
       <c r="F14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H14" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U14" s="2" t="n">
         <v>245.0</v>
@@ -4697,90 +4714,90 @@
         <v>0</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Z14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AA14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AB14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AC14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H15" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U15" s="2" t="n">
         <v>156.0</v>
@@ -4792,90 +4809,90 @@
         <v>0</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y15" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Z15" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AA15" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AB15" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AC15" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD15" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AE15" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H16" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U16" s="2" t="n">
         <v>318.0</v>
@@ -4887,90 +4904,90 @@
         <v>0</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Z16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AA16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AB16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AC16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AE16" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H17" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U17" s="2" t="n">
         <v>56.0</v>
@@ -4982,90 +4999,90 @@
         <v>0</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Z17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AA17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AB17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AC17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AE17" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H18" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U18" s="2" t="n">
         <v>596.0</v>
@@ -5077,90 +5094,90 @@
         <v>0</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Z18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AA18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AB18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AC18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AE18" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H19" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="U19" s="2" t="n">
         <v>701.0</v>
@@ -5172,28 +5189,28 @@
         <v>0</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Z19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AA19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AB19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AC19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AE19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -5225,33 +5242,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2"/>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>2.0</v>
@@ -5268,7 +5285,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>16.0</v>
@@ -5286,7 +5303,7 @@
     <row r="6"/>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>18.0</v>
@@ -5339,163 +5356,163 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" ht="45.0" customHeight="true">
       <c r="A3" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" ht="45.0" customHeight="true">
       <c r="A4" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" ht="45.0" customHeight="true">
       <c r="A5" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" ht="45.0" customHeight="true">
       <c r="A6" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" ht="45.0" customHeight="true">
       <c r="A7" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -5540,324 +5557,324 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" ht="15.0" customHeight="true">
       <c r="A4" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" ht="15.0" customHeight="true">
       <c r="A5" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" ht="15.0" customHeight="true">
       <c r="A6" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="true">
       <c r="A7" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" ht="15.0" customHeight="true">
       <c r="A8" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" ht="15.0" customHeight="true">
       <c r="A9" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" ht="15.0" customHeight="true">
       <c r="A10" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" ht="15.0" customHeight="true">
       <c r="A11" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" ht="15.0" customHeight="true">
       <c r="A12" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" ht="15.0" customHeight="true">
       <c r="A13" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" ht="15.0" customHeight="true">
       <c r="A14" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -5895,71 +5912,71 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sonarcloud: fix a number of reported issues + disable crowd control in generated conf scheduling to generate solvable solutions
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
@@ -34,10 +34,9 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t xml:space="preserve">S10-Culture: Prepare for streaming GWT
-    Dan Jones
+        <t xml:space="preserve">S04-Security: Discover AI-driven OptaPlanner
+    Hugo Rye
 PINNED BY USER
--45hard total
 </t>
       </text>
     </comment>
@@ -53,10 +52,9 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t xml:space="preserve">S10-Culture: Prepare for streaming GWT
-    Dan Jones
+        <t xml:space="preserve">S04-Security: Discover AI-driven OptaPlanner
+    Hugo Rye
 PINNED BY USER
--45hard total
 </t>
       </text>
     </comment>
@@ -72,10 +70,9 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t xml:space="preserve">S10-Culture: Prepare for streaming GWT
-    Dan Jones
+        <t xml:space="preserve">S04-Security: Discover AI-driven OptaPlanner
+    Hugo Rye
 PINNED BY USER
--45hard total
 </t>
       </text>
     </comment>
@@ -91,10 +88,9 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t xml:space="preserve">S10-Culture: Prepare for streaming GWT
-    Dan Jones
+        <t xml:space="preserve">S04-Security: Discover AI-driven OptaPlanner
+    Hugo Rye
 PINNED BY USER
--45hard total
 </t>
       </text>
     </comment>
@@ -110,11 +106,9 @@
   <commentList>
     <comment ref="B3" authorId="0">
       <text>
-        <t xml:space="preserve">S10-Culture: Prepare for streaming GWT
-    Dan Jones
+        <t xml:space="preserve">S04-Security: Discover AI-driven OptaPlanner
+    Hugo Rye
 PINNED BY USER
--45hard total
-    -45hard for 1 Crowd controls
 </t>
       </text>
     </comment>
@@ -130,11 +124,9 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t xml:space="preserve">S10-Culture: Prepare for streaming GWT
-    Dan Jones
+        <t xml:space="preserve">S04-Security: Discover AI-driven OptaPlanner
+    Hugo Rye
 PINNED BY USER
--45hard total
-    -45hard for 1 Crowd controls
 </t>
       </text>
     </comment>
@@ -148,12 +140,11 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="C6" authorId="0">
+    <comment ref="C10" authorId="0">
       <text>
-        <t xml:space="preserve">S10-Culture: Prepare for streaming GWT
-    Dan Jones
+        <t xml:space="preserve">S04-Security: Discover AI-driven OptaPlanner
+    Hugo Rye
 PINNED BY USER
--45hard total
 </t>
       </text>
     </comment>
@@ -169,10 +160,9 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t xml:space="preserve">S10-Culture: Prepare for streaming GWT
-    Dan Jones
+        <t xml:space="preserve">S04-Security: Discover AI-driven OptaPlanner
+    Hugo Rye
 PINNED BY USER
--45hard total
 </t>
       </text>
     </comment>
@@ -181,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="270">
   <si>
     <t>Conference name</t>
   </si>
@@ -687,189 +677,189 @@
     <t>Advanced containerized WildFly</t>
   </si>
   <si>
-    <t>Chad Green, Dan Jones</t>
+    <t>Chad Green, Dan Jones, Elsa King</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>WildFly</t>
+  </si>
+  <si>
+    <t>S02</t>
+  </si>
+  <si>
+    <t>Learn virtualized Spring</t>
+  </si>
+  <si>
+    <t>Culture</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>S03</t>
+  </si>
+  <si>
+    <t>Intro to serverless Drools</t>
+  </si>
+  <si>
+    <t>Drools</t>
+  </si>
+  <si>
+    <t>S04</t>
+  </si>
+  <si>
+    <t>Discover AI-driven OptaPlanner</t>
+  </si>
+  <si>
+    <t>Managers</t>
+  </si>
+  <si>
+    <t>OptaPlanner</t>
+  </si>
+  <si>
+    <t>S05</t>
+  </si>
+  <si>
+    <t>Mastering machine learning jBPM</t>
+  </si>
+  <si>
+    <t>jBPM</t>
+  </si>
+  <si>
+    <t>S06</t>
+  </si>
+  <si>
+    <t>Tuning IOT-driven Camel</t>
+  </si>
+  <si>
+    <t>Jay Watt, Amy Fox</t>
+  </si>
+  <si>
+    <t>Modern Web</t>
+  </si>
+  <si>
+    <t>Camel</t>
+  </si>
+  <si>
+    <t>S07</t>
+  </si>
+  <si>
+    <t>Building deep learning XStream</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>Programmers</t>
+  </si>
+  <si>
+    <t>XStream</t>
+  </si>
+  <si>
+    <t>S08</t>
+  </si>
+  <si>
+    <t>Securing scalable Docker</t>
+  </si>
+  <si>
+    <t>Amy Cole, Beth Fox, Chad Green</t>
   </si>
   <si>
     <t>Transportation</t>
   </si>
   <si>
-    <t>Managers</t>
-  </si>
-  <si>
-    <t>WildFly</t>
-  </si>
-  <si>
-    <t>S02</t>
-  </si>
-  <si>
-    <t>Learn virtualized Spring</t>
+    <t>Docker</t>
+  </si>
+  <si>
+    <t>S09</t>
+  </si>
+  <si>
+    <t>Debug enterprise Hibernate</t>
+  </si>
+  <si>
+    <t>Hibernate</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>Prepare for streaming GWT</t>
+  </si>
+  <si>
+    <t>Elsa King, Flo Li</t>
+  </si>
+  <si>
+    <t>GWT</t>
+  </si>
+  <si>
+    <t>S11</t>
+  </si>
+  <si>
+    <t>Understand mobile Errai</t>
+  </si>
+  <si>
+    <t>Modern Web, Security</t>
+  </si>
+  <si>
+    <t>Errai</t>
+  </si>
+  <si>
+    <t>S12</t>
+  </si>
+  <si>
+    <t>Applying modern Angular</t>
+  </si>
+  <si>
+    <t>Hugo Rye, Ivy Smith</t>
   </si>
   <si>
     <t>IoT</t>
   </si>
   <si>
-    <t>Programmers</t>
-  </si>
-  <si>
-    <t>Spring</t>
-  </si>
-  <si>
-    <t>S03</t>
-  </si>
-  <si>
-    <t>Intro to serverless Drools</t>
-  </si>
-  <si>
-    <t>Big Data, Culture</t>
-  </si>
-  <si>
-    <t>Drools</t>
-  </si>
-  <si>
-    <t>S04</t>
-  </si>
-  <si>
-    <t>Discover AI-driven OptaPlanner</t>
-  </si>
-  <si>
-    <t>Gus Poe, Hugo Rye</t>
-  </si>
-  <si>
-    <t>OptaPlanner</t>
-  </si>
-  <si>
-    <t>S05</t>
-  </si>
-  <si>
-    <t>Mastering machine learning jBPM</t>
-  </si>
-  <si>
-    <t>Middleware, Modern Web</t>
+    <t>Angular</t>
+  </si>
+  <si>
+    <t>S13</t>
+  </si>
+  <si>
+    <t>Grok distributed Weld</t>
+  </si>
+  <si>
+    <t>Cloud, Middleware</t>
   </si>
   <si>
     <t>Financial services</t>
   </si>
   <si>
-    <t>jBPM</t>
-  </si>
-  <si>
-    <t>S06</t>
-  </si>
-  <si>
-    <t>Tuning IOT-driven Camel</t>
-  </si>
-  <si>
-    <t>Government</t>
-  </si>
-  <si>
-    <t>Camel</t>
-  </si>
-  <si>
-    <t>S07</t>
-  </si>
-  <si>
-    <t>Building deep learning XStream</t>
-  </si>
-  <si>
-    <t>Amy Fox, Beth Green, Amy Cole</t>
+    <t>Weld</t>
+  </si>
+  <si>
+    <t>S14</t>
+  </si>
+  <si>
+    <t>Troubleshooting reliable RestEasy</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>RestEasy</t>
+  </si>
+  <si>
+    <t>S15</t>
+  </si>
+  <si>
+    <t>Using secure Android</t>
   </si>
   <si>
     <t>Cloud</t>
   </si>
   <si>
-    <t>XStream</t>
-  </si>
-  <si>
-    <t>S08</t>
-  </si>
-  <si>
-    <t>Securing scalable Docker</t>
-  </si>
-  <si>
-    <t>Security, Culture</t>
-  </si>
-  <si>
-    <t>Docker, Kubernetes</t>
-  </si>
-  <si>
-    <t>S09</t>
-  </si>
-  <si>
-    <t>Debug enterprise Hibernate</t>
-  </si>
-  <si>
-    <t>Culture</t>
-  </si>
-  <si>
-    <t>Telecommunications</t>
-  </si>
-  <si>
-    <t>Hibernate</t>
-  </si>
-  <si>
-    <t>S10</t>
-  </si>
-  <si>
-    <t>Prepare for streaming GWT</t>
-  </si>
-  <si>
-    <t>GWT</t>
-  </si>
-  <si>
-    <t>S11</t>
-  </si>
-  <si>
-    <t>Understand mobile Errai</t>
-  </si>
-  <si>
-    <t>Elsa King, Flo Li</t>
-  </si>
-  <si>
-    <t>Artificial Intelligence</t>
-  </si>
-  <si>
-    <t>Errai</t>
-  </si>
-  <si>
-    <t>S12</t>
-  </si>
-  <si>
-    <t>Applying modern Angular</t>
-  </si>
-  <si>
-    <t>Angular</t>
-  </si>
-  <si>
-    <t>S13</t>
-  </si>
-  <si>
-    <t>Grok distributed Weld</t>
-  </si>
-  <si>
-    <t>Middleware, Security</t>
-  </si>
-  <si>
-    <t>Weld</t>
-  </si>
-  <si>
-    <t>S14</t>
-  </si>
-  <si>
-    <t>Troubleshooting reliable RestEasy</t>
-  </si>
-  <si>
-    <t>Mobile, Culture</t>
-  </si>
-  <si>
-    <t>RestEasy</t>
-  </si>
-  <si>
-    <t>S15</t>
-  </si>
-  <si>
-    <t>Using secure Android</t>
-  </si>
-  <si>
     <t>Android</t>
   </si>
   <si>
@@ -879,9 +869,6 @@
     <t>Deliver stable Tensorflow</t>
   </si>
   <si>
-    <t>Cloud, Culture</t>
-  </si>
-  <si>
     <t>Tensorflow</t>
   </si>
   <si>
@@ -891,16 +878,13 @@
     <t>Implement platform-independent VertX</t>
   </si>
   <si>
-    <t>Middleware</t>
-  </si>
-  <si>
     <t>VertX</t>
   </si>
   <si>
     <t>Score</t>
   </si>
   <si>
-    <t>-34init/-45hard</t>
+    <t>-34init</t>
   </si>
   <si>
     <t>Count</t>
@@ -918,14 +902,14 @@
     <t>Total</t>
   </si>
   <si>
-    <t>S10: Prepare for streaming GWT
-  Dan Jones</t>
+    <t>S04: Discover AI-driven OptaPlanner
+  Hugo Rye</t>
   </si>
   <si>
     <t>Speaker</t>
   </si>
   <si>
-    <t>S10 @ R 1</t>
+    <t>S04 @ R 1</t>
   </si>
   <si>
     <t>Theme track tag</t>
@@ -937,13 +921,13 @@
     <t>Audience type</t>
   </si>
   <si>
-    <t>1</t>
+    <t>3</t>
   </si>
   <si>
     <t>Content tag</t>
   </si>
   <si>
-    <t>S10 (level 1)</t>
+    <t>S04 (level 3)</t>
   </si>
   <si>
     <t>Constraint name</t>
@@ -982,9 +966,6 @@
     <t>1hard</t>
   </si>
   <si>
-    <t>-45hard</t>
-  </si>
-  <si>
     <t>1medium</t>
   </si>
   <si>
@@ -1000,8 +981,8 @@
     <t>1soft</t>
   </si>
   <si>
-    <t>Prepare for streaming GWT
-Dan Jones</t>
+    <t>Discover AI-driven OptaPlanner
+Hugo Rye</t>
   </si>
 </sst>
 </file>
@@ -1761,7 +1742,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>105</v>
@@ -1839,7 +1820,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>105</v>
@@ -1862,13 +1843,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>93</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>93</v>
@@ -1964,13 +1945,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>93</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>93</v>
@@ -2009,7 +1990,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="11.78515625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="12.62109375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.86328125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="11.9140625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.86328125" customWidth="true" bestFit="true"/>
@@ -2043,7 +2024,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>105</v>
@@ -2066,13 +2047,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>210</v>
+        <v>181</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>93</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>93</v>
@@ -2174,7 +2155,7 @@
         <v>93</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>93</v>
@@ -2204,7 +2185,7 @@
   <sheetPr>
     <tabColor rgb="FCE94F"/>
   </sheetPr>
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:H80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" ySplit="3.0" state="frozen" topLeftCell="B4" activePane="bottomRight"/>
@@ -2216,7 +2197,7 @@
     <col min="1" max="1" width="35.140625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="17.34375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.65234375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="8.0703125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="6.0859375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="1.0546875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="12.296875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="12.9296875" customWidth="true" bestFit="true"/>
@@ -2224,39 +2205,39 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2"/>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2269,13 +2250,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6">
@@ -2283,13 +2264,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7">
@@ -2297,13 +2278,13 @@
         <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8">
@@ -2311,13 +2292,13 @@
         <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9">
@@ -2325,13 +2306,13 @@
         <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10">
@@ -2339,13 +2320,13 @@
         <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11">
@@ -2353,13 +2334,13 @@
         <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="12">
@@ -2367,13 +2348,13 @@
         <v>36</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13">
@@ -2381,13 +2362,13 @@
         <v>30</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14">
@@ -2395,13 +2376,13 @@
         <v>34</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="15">
@@ -2409,13 +2390,13 @@
         <v>28</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16">
@@ -2423,13 +2404,13 @@
         <v>21</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17">
@@ -2437,13 +2418,13 @@
         <v>39</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18">
@@ -2451,13 +2432,13 @@
         <v>33</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19">
@@ -2465,13 +2446,13 @@
         <v>38</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20">
@@ -2479,13 +2460,13 @@
         <v>32</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21">
@@ -2493,13 +2474,13 @@
         <v>40</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22">
@@ -2507,13 +2488,13 @@
         <v>62</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23">
@@ -2521,13 +2502,13 @@
         <v>78</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="24">
@@ -2535,13 +2516,13 @@
         <v>71</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25">
@@ -2549,13 +2530,13 @@
         <v>80</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="26">
@@ -2563,13 +2544,13 @@
         <v>74</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27">
@@ -2577,13 +2558,13 @@
         <v>82</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28">
@@ -2591,13 +2572,13 @@
         <v>76</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="29">
@@ -2605,13 +2586,13 @@
         <v>83</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30">
@@ -2619,13 +2600,13 @@
         <v>77</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31">
@@ -2633,13 +2614,13 @@
         <v>60</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="32">
@@ -2647,13 +2628,13 @@
         <v>65</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33">
@@ -2661,13 +2642,13 @@
         <v>69</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C33" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="34">
@@ -2675,13 +2656,13 @@
         <v>43</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="35">
@@ -2689,13 +2670,13 @@
         <v>67</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="36">
@@ -2703,13 +2684,13 @@
         <v>50</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="37">
@@ -2717,13 +2698,13 @@
         <v>46</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="38">
@@ -2731,13 +2712,13 @@
         <v>48</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="39">
@@ -2745,13 +2726,13 @@
         <v>58</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="40">
@@ -2759,13 +2740,13 @@
         <v>52</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="41">
@@ -2773,89 +2754,90 @@
         <v>55</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C41" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="42"/>
     <row r="43"/>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C44" s="2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>208</v>
+      <c r="A45" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C45" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="C46" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C47" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="C48" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>265</v>
@@ -2864,455 +2846,441 @@
         <v>0.0</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C50" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C51" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C52" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C53" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C54" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C55" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C56" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="C57" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C58" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C59" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C60" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C61" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C62" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C63" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C64" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C65" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C66" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C67" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C68" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C69" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C70" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C71" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C72" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C73" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C74" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C75" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C76" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C77" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C78" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C79" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C80" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="C81" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -3359,8 +3327,8 @@
       <c r="A3" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>272</v>
+      <c r="B3" s="13" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="4" ht="45.0" customHeight="true">
@@ -4510,12 +4478,12 @@
     <col min="1" max="1" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="36.7734375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="9.41796875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="29.4140625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="24.78515625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="19.625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="30.52734375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="21.19921875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="16.515625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="16.4453125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="14.4375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="18.64453125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.6640625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="9.7109375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="21.69921875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="22.09765625" customWidth="true" bestFit="true"/>
@@ -4700,7 +4668,7 @@
         <v>623.0</v>
       </c>
       <c r="V2" s="2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W2" s="2" t="b">
         <v>0</v>
@@ -4744,19 +4712,19 @@
         <v>168</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>169</v>
+        <v>93</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>165</v>
@@ -4792,7 +4760,7 @@
         <v>93</v>
       </c>
       <c r="U3" s="2" t="n">
-        <v>291.0</v>
+        <v>942.0</v>
       </c>
       <c r="V3" s="2" t="n">
         <v>0.0</v>
@@ -4827,31 +4795,31 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>165</v>
@@ -4887,7 +4855,7 @@
         <v>93</v>
       </c>
       <c r="U4" s="2" t="n">
-        <v>214.0</v>
+        <v>293.0</v>
       </c>
       <c r="V4" s="2" t="n">
         <v>0.0</v>
@@ -4922,31 +4890,31 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>93</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>165</v>
@@ -4982,10 +4950,10 @@
         <v>93</v>
       </c>
       <c r="U5" s="2" t="n">
-        <v>761.0</v>
+        <v>82.0</v>
       </c>
       <c r="V5" s="2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W5" s="2" t="b">
         <v>0</v>
@@ -5017,31 +4985,31 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>93</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>165</v>
@@ -5077,25 +5045,25 @@
         <v>93</v>
       </c>
       <c r="U6" s="2" t="n">
-        <v>388.0</v>
+        <v>579.0</v>
       </c>
       <c r="V6" s="2" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="W6" s="2" t="b">
-        <v>0</v>
+        <v>0.0</v>
+      </c>
+      <c r="W6" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="AB6" s="2" t="s">
         <v>93</v>
@@ -5112,10 +5080,10 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>95</v>
@@ -5124,19 +5092,19 @@
         <v>134</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>188</v>
+        <v>93</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="H7" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>165</v>
@@ -5172,10 +5140,10 @@
         <v>93</v>
       </c>
       <c r="U7" s="2" t="n">
-        <v>798.0</v>
+        <v>377.0</v>
       </c>
       <c r="V7" s="2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W7" s="2" t="b">
         <v>0</v>
@@ -5207,31 +5175,31 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>135</v>
+        <v>187</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>192</v>
+        <v>93</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>165</v>
@@ -5267,10 +5235,10 @@
         <v>93</v>
       </c>
       <c r="U8" s="2" t="n">
-        <v>401.0</v>
+        <v>196.0</v>
       </c>
       <c r="V8" s="2" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="W8" s="2" t="b">
         <v>0</v>
@@ -5302,31 +5270,31 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>196</v>
+        <v>137</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>93</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>170</v>
+        <v>193</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>165</v>
@@ -5362,10 +5330,10 @@
         <v>93</v>
       </c>
       <c r="U9" s="2" t="n">
-        <v>720.0</v>
+        <v>401.0</v>
       </c>
       <c r="V9" s="2" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="W9" s="2" t="b">
         <v>0</v>
@@ -5397,31 +5365,31 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>127</v>
+        <v>197</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>201</v>
+        <v>169</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>93</v>
+        <v>198</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="H10" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>165</v>
@@ -5457,10 +5425,10 @@
         <v>93</v>
       </c>
       <c r="U10" s="2" t="n">
-        <v>55.0</v>
+        <v>226.0</v>
       </c>
       <c r="V10" s="2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W10" s="2" t="b">
         <v>0</v>
@@ -5492,31 +5460,31 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>205</v>
+        <v>169</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>206</v>
+        <v>93</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>163</v>
+        <v>193</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>165</v>
@@ -5552,7 +5520,7 @@
         <v>93</v>
       </c>
       <c r="U11" s="2" t="n">
-        <v>333.0</v>
+        <v>361.0</v>
       </c>
       <c r="V11" s="2" t="n">
         <v>0.0</v>
@@ -5587,31 +5555,31 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>129</v>
+        <v>205</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>205</v>
+        <v>169</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>93</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="H12" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>165</v>
@@ -5647,25 +5615,25 @@
         <v>93</v>
       </c>
       <c r="U12" s="2" t="n">
-        <v>546.0</v>
+        <v>526.0</v>
       </c>
       <c r="V12" s="2" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="W12" s="6" t="b">
-        <v>1</v>
+        <v>0.0</v>
+      </c>
+      <c r="W12" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA12" s="2" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="AB12" s="2" t="s">
         <v>93</v>
@@ -5682,31 +5650,31 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>213</v>
+        <v>132</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>169</v>
+        <v>93</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>163</v>
+        <v>193</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>165</v>
@@ -5742,10 +5710,10 @@
         <v>93</v>
       </c>
       <c r="U13" s="2" t="n">
-        <v>785.0</v>
+        <v>185.0</v>
       </c>
       <c r="V13" s="2" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="W13" s="2" t="b">
         <v>0</v>
@@ -5777,16 +5745,16 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>132</v>
+        <v>213</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>214</v>
@@ -5795,13 +5763,13 @@
         <v>93</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>170</v>
+        <v>193</v>
       </c>
       <c r="H14" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>165</v>
@@ -5837,10 +5805,10 @@
         <v>93</v>
       </c>
       <c r="U14" s="2" t="n">
-        <v>245.0</v>
+        <v>405.0</v>
       </c>
       <c r="V14" s="2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W14" s="2" t="b">
         <v>0</v>
@@ -5872,31 +5840,31 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>188</v>
+        <v>219</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>163</v>
+        <v>193</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>165</v>
@@ -5932,10 +5900,10 @@
         <v>93</v>
       </c>
       <c r="U15" s="2" t="n">
-        <v>156.0</v>
+        <v>340.0</v>
       </c>
       <c r="V15" s="2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W15" s="2" t="b">
         <v>0</v>
@@ -5967,31 +5935,31 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="H16" s="2" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>226</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>165</v>
@@ -6027,10 +5995,10 @@
         <v>93</v>
       </c>
       <c r="U16" s="2" t="n">
-        <v>318.0</v>
+        <v>1.0</v>
       </c>
       <c r="V16" s="2" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="W16" s="2" t="b">
         <v>0</v>
@@ -6062,28 +6030,28 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>228</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>174</v>
+        <v>228</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>93</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>163</v>
+        <v>193</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>229</v>
@@ -6122,10 +6090,10 @@
         <v>93</v>
       </c>
       <c r="U17" s="2" t="n">
-        <v>56.0</v>
+        <v>824.0</v>
       </c>
       <c r="V17" s="2" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="W17" s="2" t="b">
         <v>0</v>
@@ -6166,22 +6134,22 @@
         <v>95</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="H18" s="2" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>233</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>165</v>
@@ -6217,10 +6185,10 @@
         <v>93</v>
       </c>
       <c r="U18" s="2" t="n">
-        <v>596.0</v>
+        <v>318.0</v>
       </c>
       <c r="V18" s="2" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="W18" s="2" t="b">
         <v>0</v>
@@ -6252,31 +6220,31 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>235</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>236</v>
+        <v>169</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>93</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="H19" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>165</v>
@@ -6312,10 +6280,10 @@
         <v>93</v>
       </c>
       <c r="U19" s="2" t="n">
-        <v>701.0</v>
+        <v>138.0</v>
       </c>
       <c r="V19" s="2" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="W19" s="2" t="b">
         <v>0</v>
@@ -6366,7 +6334,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="9.4453125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="14.7265625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="6.83984375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="16.22265625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="13.59375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.30078125" customWidth="true" bestFit="true"/>
@@ -6374,10 +6342,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2"/>
@@ -6386,16 +6354,16 @@
         <v>140</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="4">
@@ -6435,7 +6403,7 @@
     <row r="6"/>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>18.0</v>
@@ -6540,7 +6508,7 @@
         <v>93</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>93</v>
@@ -6712,7 +6680,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>105</v>
@@ -6809,8 +6777,8 @@
       <c r="B6" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>247</v>
+      <c r="C6" s="10" t="s">
+        <v>93</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>93</v>
@@ -6901,8 +6869,8 @@
       <c r="B10" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>93</v>
+      <c r="C10" s="6" t="s">
+        <v>245</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>93</v>
@@ -7067,7 +7035,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>105</v>
@@ -7090,13 +7058,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>205</v>
+        <v>169</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>93</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>93</v>

</xml_diff>

<commit_message>
Add room tag sets
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/18talks-6timeslots-5rooms.xlsx
@@ -304,7 +304,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="283">
   <si>
     <t>Conference name</t>
   </si>
@@ -879,9 +879,6 @@
     <t>jBPM</t>
   </si>
   <si>
-    <t>Large</t>
-  </si>
-  <si>
     <t>S06</t>
   </si>
   <si>
@@ -1012,9 +1009,6 @@
   </si>
   <si>
     <t>Tensorflow</t>
-  </si>
-  <si>
-    <t>Large, Recorded</t>
   </si>
   <si>
     <t>S17</t>
@@ -1914,7 +1908,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>106</v>
@@ -1992,7 +1986,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>106</v>
@@ -2018,10 +2012,10 @@
         <v>164</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>93</v>
@@ -2117,13 +2111,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>93</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>93</v>
@@ -2140,10 +2134,10 @@
     </row>
     <row r="4" ht="15.0" customHeight="true">
       <c r="A4" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>93</v>
@@ -2219,7 +2213,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>106</v>
@@ -2242,13 +2236,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>93</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>93</v>
@@ -2265,10 +2259,10 @@
     </row>
     <row r="4" ht="15.0" customHeight="true">
       <c r="A4" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>93</v>
@@ -2288,10 +2282,10 @@
     </row>
     <row r="5" ht="15.0" customHeight="true">
       <c r="A5" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>93</v>
@@ -2393,10 +2387,10 @@
         <v>166</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>93</v>
@@ -2446,39 +2440,39 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2"/>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2491,13 +2485,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6">
@@ -2505,13 +2499,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7">
@@ -2519,13 +2513,13 @@
         <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8">
@@ -2533,13 +2527,13 @@
         <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9">
@@ -2547,13 +2541,13 @@
         <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10">
@@ -2561,13 +2555,13 @@
         <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11">
@@ -2575,13 +2569,13 @@
         <v>37</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12">
@@ -2589,13 +2583,13 @@
         <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13">
@@ -2603,13 +2597,13 @@
         <v>35</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14">
@@ -2617,13 +2611,13 @@
         <v>29</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15">
@@ -2631,13 +2625,13 @@
         <v>21</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16">
@@ -2645,13 +2639,13 @@
         <v>40</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17">
@@ -2659,13 +2653,13 @@
         <v>34</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18">
@@ -2673,13 +2667,13 @@
         <v>39</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19">
@@ -2687,13 +2681,13 @@
         <v>33</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="20">
@@ -2701,13 +2695,13 @@
         <v>41</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="21">
@@ -2715,13 +2709,13 @@
         <v>62</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22">
@@ -2729,13 +2723,13 @@
         <v>78</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="23">
@@ -2743,13 +2737,13 @@
         <v>71</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="24">
@@ -2757,13 +2751,13 @@
         <v>80</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="25">
@@ -2771,13 +2765,13 @@
         <v>74</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="26">
@@ -2785,13 +2779,13 @@
         <v>82</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="27">
@@ -2799,13 +2793,13 @@
         <v>76</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="28">
@@ -2813,13 +2807,13 @@
         <v>83</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="29">
@@ -2827,13 +2821,13 @@
         <v>77</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="30">
@@ -2841,13 +2835,13 @@
         <v>60</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="31">
@@ -2855,13 +2849,13 @@
         <v>65</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="32">
@@ -2869,13 +2863,13 @@
         <v>69</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="33">
@@ -2883,13 +2877,13 @@
         <v>44</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C33" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34">
@@ -2897,13 +2891,13 @@
         <v>67</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="35">
@@ -2911,13 +2905,13 @@
         <v>51</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="36">
@@ -2925,13 +2919,13 @@
         <v>47</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="37">
@@ -2939,13 +2933,13 @@
         <v>49</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="38">
@@ -2953,13 +2947,13 @@
         <v>58</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="39">
@@ -2967,13 +2961,13 @@
         <v>53</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="40">
@@ -2981,13 +2975,13 @@
         <v>56</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="41">
@@ -2995,13 +2989,13 @@
         <v>26</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C41" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="42"/>
@@ -3011,13 +3005,13 @@
         <v>49</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C44" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="45">
@@ -3027,10 +3021,10 @@
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="46">
@@ -3038,13 +3032,13 @@
         <v>47</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C46" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="47">
@@ -3054,10 +3048,10 @@
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="48">
@@ -3065,13 +3059,13 @@
         <v>56</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C48" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="49">
@@ -3081,10 +3075,10 @@
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="50">
@@ -3092,13 +3086,13 @@
         <v>58</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C50" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="51">
@@ -3106,13 +3100,13 @@
         <v>53</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C51" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="52">
@@ -3120,13 +3114,13 @@
         <v>24</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C52" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="53">
@@ -3134,13 +3128,13 @@
         <v>60</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C53" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="54">
@@ -3148,13 +3142,13 @@
         <v>62</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C54" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="55">
@@ -3162,13 +3156,13 @@
         <v>26</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C55" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="56">
@@ -3176,13 +3170,13 @@
         <v>65</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C56" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="57">
@@ -3190,13 +3184,13 @@
         <v>69</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C57" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="58">
@@ -3204,13 +3198,13 @@
         <v>44</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C58" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="59">
@@ -3218,13 +3212,13 @@
         <v>41</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C59" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="60">
@@ -3232,13 +3226,13 @@
         <v>10</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C60" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="61">
@@ -3246,13 +3240,13 @@
         <v>7</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C61" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="62">
@@ -3260,13 +3254,13 @@
         <v>67</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C62" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="63">
@@ -3274,13 +3268,13 @@
         <v>51</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C63" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="64">
@@ -3288,13 +3282,13 @@
         <v>16</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C64" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="65">
@@ -3302,13 +3296,13 @@
         <v>78</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C65" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="66">
@@ -3316,13 +3310,13 @@
         <v>71</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C66" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="67">
@@ -3330,13 +3324,13 @@
         <v>37</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C67" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="68">
@@ -3344,13 +3338,13 @@
         <v>31</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C68" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="69">
@@ -3358,13 +3352,13 @@
         <v>35</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C69" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="70">
@@ -3372,13 +3366,13 @@
         <v>29</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C70" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="71">
@@ -3386,13 +3380,13 @@
         <v>13</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C71" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="72">
@@ -3400,13 +3394,13 @@
         <v>80</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C72" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="73">
@@ -3414,13 +3408,13 @@
         <v>74</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C73" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="74">
@@ -3428,13 +3422,13 @@
         <v>21</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C74" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="75">
@@ -3442,13 +3436,13 @@
         <v>82</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C75" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="76">
@@ -3456,13 +3450,13 @@
         <v>76</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C76" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="77">
@@ -3470,13 +3464,13 @@
         <v>19</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C77" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="78">
@@ -3484,13 +3478,13 @@
         <v>40</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C78" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="79">
@@ -3498,13 +3492,13 @@
         <v>34</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C79" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="80">
@@ -3512,13 +3506,13 @@
         <v>39</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C80" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="81">
@@ -3526,13 +3520,13 @@
         <v>33</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C81" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="82">
@@ -3540,13 +3534,13 @@
         <v>83</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C82" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="83">
@@ -3554,13 +3548,13 @@
         <v>77</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C83" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -3607,7 +3601,7 @@
         <v>93</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" ht="45.0" customHeight="true">
@@ -3615,7 +3609,7 @@
         <v>107</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -5046,13 +5040,13 @@
         <v>93</v>
       </c>
       <c r="P3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>93</v>
@@ -5141,7 +5135,7 @@
         <v>93</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>93</v>
@@ -5236,7 +5230,7 @@
         <v>93</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>93</v>
@@ -5426,7 +5420,7 @@
         <v>93</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>191</v>
+        <v>93</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>93</v>
@@ -5476,10 +5470,10 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>193</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>95</v>
@@ -5500,7 +5494,7 @@
         <v>3.0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>166</v>
@@ -5521,7 +5515,7 @@
         <v>93</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>191</v>
+        <v>93</v>
       </c>
       <c r="Q8" s="2" t="s">
         <v>93</v>
@@ -5571,10 +5565,10 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>196</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>95</v>
@@ -5583,10 +5577,10 @@
         <v>137</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>170</v>
@@ -5595,7 +5589,7 @@
         <v>3.0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>166</v>
@@ -5616,7 +5610,7 @@
         <v>93</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>93</v>
@@ -5666,19 +5660,19 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>203</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>93</v>
@@ -5690,7 +5684,7 @@
         <v>3.0</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>166</v>
@@ -5711,7 +5705,7 @@
         <v>93</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>191</v>
+        <v>93</v>
       </c>
       <c r="Q10" s="2" t="s">
         <v>93</v>
@@ -5761,19 +5755,19 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>174</v>
@@ -5785,7 +5779,7 @@
         <v>3.0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>166</v>
@@ -5856,16 +5850,16 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>163</v>
@@ -5880,7 +5874,7 @@
         <v>1.0</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>166</v>
@@ -5951,19 +5945,19 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>214</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>93</v>
@@ -5975,7 +5969,7 @@
         <v>3.0</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>166</v>
@@ -5996,7 +5990,7 @@
         <v>93</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="Q13" s="2" t="s">
         <v>93</v>
@@ -6005,7 +5999,7 @@
         <v>93</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="T13" s="2" t="s">
         <v>93</v>
@@ -6046,10 +6040,10 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>219</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>95</v>
@@ -6058,7 +6052,7 @@
         <v>134</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>93</v>
@@ -6070,7 +6064,7 @@
         <v>3.0</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>166</v>
@@ -6141,10 +6135,10 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>95</v>
@@ -6165,7 +6159,7 @@
         <v>3.0</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>166</v>
@@ -6236,10 +6230,10 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>226</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>95</v>
@@ -6248,7 +6242,7 @@
         <v>136</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>93</v>
@@ -6260,7 +6254,7 @@
         <v>2.0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>166</v>
@@ -6278,16 +6272,16 @@
         <v>93</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>191</v>
+        <v>93</v>
       </c>
       <c r="Q16" s="2" t="s">
         <v>93</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="S16" s="2" t="s">
         <v>93</v>
@@ -6331,16 +6325,16 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>179</v>
@@ -6355,7 +6349,7 @@
         <v>1.0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>166</v>
@@ -6376,7 +6370,7 @@
         <v>93</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>191</v>
+        <v>93</v>
       </c>
       <c r="Q17" s="2" t="s">
         <v>93</v>
@@ -6426,10 +6420,10 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>95</v>
@@ -6450,7 +6444,7 @@
         <v>2.0</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>166</v>
@@ -6471,7 +6465,7 @@
         <v>93</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>236</v>
+        <v>93</v>
       </c>
       <c r="Q18" s="2" t="s">
         <v>93</v>
@@ -6521,19 +6515,19 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>93</v>
@@ -6545,7 +6539,7 @@
         <v>2.0</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>166</v>
@@ -6566,7 +6560,7 @@
         <v>93</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>236</v>
+        <v>93</v>
       </c>
       <c r="Q19" s="2" t="s">
         <v>93</v>
@@ -6643,10 +6637,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2"/>
@@ -6655,16 +6649,16 @@
         <v>141</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="4">
@@ -6704,7 +6698,7 @@
     <row r="6"/>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>18.0</v>
@@ -6809,7 +6803,7 @@
         <v>93</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>93</v>
@@ -6898,7 +6892,7 @@
         <v>118</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -6978,7 +6972,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>106</v>
@@ -7004,7 +6998,7 @@
         <v>127</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -7023,7 +7017,7 @@
         <v>128</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -7068,7 +7062,7 @@
         <v>93</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>93</v>
@@ -7091,7 +7085,7 @@
         <v>93</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>93</v>
@@ -7327,7 +7321,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>106</v>
@@ -7353,10 +7347,10 @@
         <v>163</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>93</v>

</xml_diff>